<commit_message>
Change config files and add algorithms results
</commit_message>
<xml_diff>
--- a/algorithms_results.xlsx
+++ b/algorithms_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Studia\mgr\praca_magisterska\auth-smile-classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE4942F-02AD-4FD2-B43F-D279AF66C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8374F4-5D12-4D2A-BDE3-39A1397EAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-144" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="213">
   <si>
     <t>scaled</t>
   </si>
@@ -670,6 +670,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>BRWI 2</t>
+  </si>
+  <si>
+    <t>BRWI 3</t>
   </si>
 </sst>
 </file>
@@ -682,12 +688,20 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -847,51 +861,56 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -900,8 +919,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
@@ -1183,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AL210"/>
+  <dimension ref="A2:AL236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="F223" sqref="F223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1200,11 +1224,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -1218,7 +1242,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -1238,7 +1262,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="30"/>
+      <c r="A5" s="33"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -1256,7 +1280,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="30"/>
+      <c r="A6" s="33"/>
       <c r="B6">
         <v>2</v>
       </c>
@@ -1274,7 +1298,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="30"/>
+      <c r="A7" s="33"/>
       <c r="B7">
         <v>3</v>
       </c>
@@ -1292,7 +1316,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="30"/>
+      <c r="A8" s="33"/>
       <c r="B8">
         <v>4</v>
       </c>
@@ -1310,7 +1334,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="30"/>
+      <c r="A9" s="33"/>
       <c r="B9">
         <v>5</v>
       </c>
@@ -1802,11 +1826,11 @@
       </c>
     </row>
     <row r="59" spans="3:25">
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
     </row>
     <row r="60" spans="3:25">
       <c r="E60" s="1" t="s">
@@ -1820,7 +1844,7 @@
       </c>
     </row>
     <row r="61" spans="3:25">
-      <c r="C61" s="29" t="s">
+      <c r="C61" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="1">
@@ -1843,7 +1867,7 @@
       </c>
     </row>
     <row r="62" spans="3:25">
-      <c r="C62" s="29"/>
+      <c r="C62" s="32"/>
       <c r="D62" s="1">
         <v>1</v>
       </c>
@@ -1864,7 +1888,7 @@
       </c>
     </row>
     <row r="63" spans="3:25">
-      <c r="C63" s="29"/>
+      <c r="C63" s="32"/>
       <c r="D63" s="1">
         <v>2</v>
       </c>
@@ -1882,7 +1906,7 @@
       </c>
     </row>
     <row r="64" spans="3:25">
-      <c r="C64" s="29"/>
+      <c r="C64" s="32"/>
       <c r="D64" s="1">
         <v>3</v>
       </c>
@@ -1903,7 +1927,7 @@
       </c>
     </row>
     <row r="65" spans="3:9">
-      <c r="C65" s="29"/>
+      <c r="C65" s="32"/>
       <c r="D65" s="1">
         <v>4</v>
       </c>
@@ -1921,7 +1945,7 @@
       </c>
     </row>
     <row r="66" spans="3:9">
-      <c r="C66" s="29"/>
+      <c r="C66" s="32"/>
       <c r="D66" s="1">
         <v>5</v>
       </c>
@@ -2030,11 +2054,11 @@
       </c>
     </row>
     <row r="80" spans="3:9">
-      <c r="E80" s="28" t="s">
+      <c r="E80" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
     </row>
     <row r="81" spans="3:33">
       <c r="E81" s="1" t="s">
@@ -2048,7 +2072,7 @@
       </c>
     </row>
     <row r="82" spans="3:33">
-      <c r="C82" s="29" t="s">
+      <c r="C82" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="1">
@@ -2068,7 +2092,7 @@
       </c>
     </row>
     <row r="83" spans="3:33">
-      <c r="C83" s="30"/>
+      <c r="C83" s="33"/>
       <c r="D83" s="1">
         <v>1</v>
       </c>
@@ -2086,7 +2110,7 @@
       </c>
     </row>
     <row r="84" spans="3:33">
-      <c r="C84" s="30"/>
+      <c r="C84" s="33"/>
       <c r="D84" s="1">
         <v>2</v>
       </c>
@@ -2104,7 +2128,7 @@
       </c>
     </row>
     <row r="85" spans="3:33">
-      <c r="C85" s="30"/>
+      <c r="C85" s="33"/>
       <c r="D85" s="1">
         <v>3</v>
       </c>
@@ -2122,7 +2146,7 @@
       </c>
     </row>
     <row r="86" spans="3:33">
-      <c r="C86" s="30"/>
+      <c r="C86" s="33"/>
       <c r="D86" s="1">
         <v>4</v>
       </c>
@@ -2140,7 +2164,7 @@
       </c>
     </row>
     <row r="87" spans="3:33">
-      <c r="C87" s="30"/>
+      <c r="C87" s="33"/>
       <c r="D87" s="1">
         <v>5</v>
       </c>
@@ -2352,11 +2376,11 @@
       </c>
     </row>
     <row r="101" spans="3:33">
-      <c r="E101" s="28" t="s">
+      <c r="E101" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
       <c r="H101" t="s">
         <v>113</v>
       </c>
@@ -2388,7 +2412,7 @@
       </c>
     </row>
     <row r="103" spans="3:33">
-      <c r="C103" s="29" t="s">
+      <c r="C103" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="1">
@@ -2406,7 +2430,7 @@
       </c>
     </row>
     <row r="104" spans="3:33">
-      <c r="C104" s="30"/>
+      <c r="C104" s="33"/>
       <c r="D104" s="1">
         <v>1</v>
       </c>
@@ -2422,7 +2446,7 @@
       </c>
     </row>
     <row r="105" spans="3:33">
-      <c r="C105" s="30"/>
+      <c r="C105" s="33"/>
       <c r="D105" s="1">
         <v>2</v>
       </c>
@@ -2438,7 +2462,7 @@
       </c>
     </row>
     <row r="106" spans="3:33">
-      <c r="C106" s="30"/>
+      <c r="C106" s="33"/>
       <c r="D106" s="1">
         <v>3</v>
       </c>
@@ -2454,7 +2478,7 @@
       </c>
     </row>
     <row r="107" spans="3:33">
-      <c r="C107" s="30"/>
+      <c r="C107" s="33"/>
       <c r="D107" s="1">
         <v>4</v>
       </c>
@@ -2470,7 +2494,7 @@
       </c>
     </row>
     <row r="108" spans="3:33">
-      <c r="C108" s="30"/>
+      <c r="C108" s="33"/>
       <c r="D108" s="1">
         <v>5</v>
       </c>
@@ -2695,11 +2719,11 @@
       </c>
     </row>
     <row r="122" spans="3:38">
-      <c r="E122" s="28" t="s">
+      <c r="E122" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F122" s="28"/>
-      <c r="G122" s="28"/>
+      <c r="F122" s="31"/>
+      <c r="G122" s="31"/>
       <c r="H122" t="s">
         <v>133</v>
       </c>
@@ -2734,7 +2758,7 @@
       </c>
     </row>
     <row r="124" spans="3:38">
-      <c r="C124" s="29" t="s">
+      <c r="C124" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="1">
@@ -2752,7 +2776,7 @@
       </c>
     </row>
     <row r="125" spans="3:38">
-      <c r="C125" s="30"/>
+      <c r="C125" s="33"/>
       <c r="D125" s="1">
         <v>1</v>
       </c>
@@ -2768,7 +2792,7 @@
       </c>
     </row>
     <row r="126" spans="3:38">
-      <c r="C126" s="30"/>
+      <c r="C126" s="33"/>
       <c r="D126" s="1">
         <v>2</v>
       </c>
@@ -2784,7 +2808,7 @@
       </c>
     </row>
     <row r="127" spans="3:38">
-      <c r="C127" s="30"/>
+      <c r="C127" s="33"/>
       <c r="D127" s="1">
         <v>3</v>
       </c>
@@ -2800,7 +2824,7 @@
       </c>
     </row>
     <row r="128" spans="3:38">
-      <c r="C128" s="30"/>
+      <c r="C128" s="33"/>
       <c r="D128" s="1">
         <v>4</v>
       </c>
@@ -2816,7 +2840,7 @@
       </c>
     </row>
     <row r="129" spans="3:22">
-      <c r="C129" s="30"/>
+      <c r="C129" s="33"/>
       <c r="D129" s="1">
         <v>5</v>
       </c>
@@ -2963,11 +2987,11 @@
       </c>
     </row>
     <row r="143" spans="3:22">
-      <c r="E143" s="28" t="s">
+      <c r="E143" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F143" s="28"/>
-      <c r="G143" s="28"/>
+      <c r="F143" s="31"/>
+      <c r="G143" s="31"/>
       <c r="L143" t="s">
         <v>154</v>
       </c>
@@ -2990,14 +3014,14 @@
       </c>
     </row>
     <row r="145" spans="3:24">
-      <c r="C145" s="29" t="s">
+      <c r="C145" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="1">
         <v>0</v>
       </c>
       <c r="E145" s="10"/>
-      <c r="F145" s="32">
+      <c r="F145" s="29">
         <v>0.70526315789473604</v>
       </c>
       <c r="G145" s="12">
@@ -3008,7 +3032,7 @@
       </c>
     </row>
     <row r="146" spans="3:24">
-      <c r="C146" s="30"/>
+      <c r="C146" s="33"/>
       <c r="D146" s="1">
         <v>1</v>
       </c>
@@ -3024,7 +3048,7 @@
       </c>
     </row>
     <row r="147" spans="3:24">
-      <c r="C147" s="30"/>
+      <c r="C147" s="33"/>
       <c r="D147" s="1">
         <v>2</v>
       </c>
@@ -3040,7 +3064,7 @@
       </c>
     </row>
     <row r="148" spans="3:24">
-      <c r="C148" s="30"/>
+      <c r="C148" s="33"/>
       <c r="D148" s="1">
         <v>3</v>
       </c>
@@ -3056,7 +3080,7 @@
       </c>
     </row>
     <row r="149" spans="3:24">
-      <c r="C149" s="30"/>
+      <c r="C149" s="33"/>
       <c r="D149" s="1">
         <v>4</v>
       </c>
@@ -3072,7 +3096,7 @@
       </c>
     </row>
     <row r="150" spans="3:24">
-      <c r="C150" s="30"/>
+      <c r="C150" s="33"/>
       <c r="D150" s="1">
         <v>5</v>
       </c>
@@ -3240,9 +3264,9 @@
       </c>
     </row>
     <row r="164" spans="3:29">
-      <c r="E164" s="28"/>
-      <c r="F164" s="28"/>
-      <c r="G164" s="28"/>
+      <c r="E164" s="31"/>
+      <c r="F164" s="31"/>
+      <c r="G164" s="31"/>
     </row>
     <row r="165" spans="3:29" ht="15.75" thickBot="1">
       <c r="E165" t="s">
@@ -3253,7 +3277,7 @@
       </c>
     </row>
     <row r="166" spans="3:29">
-      <c r="C166" s="29"/>
+      <c r="C166" s="32"/>
       <c r="D166" s="1"/>
       <c r="E166" s="5">
         <v>0.65587043762206998</v>
@@ -3269,7 +3293,7 @@
       </c>
     </row>
     <row r="167" spans="3:29">
-      <c r="C167" s="30"/>
+      <c r="C167" s="33"/>
       <c r="D167" s="1"/>
       <c r="E167" s="5">
         <v>0.70445346832275302</v>
@@ -3294,7 +3318,7 @@
       </c>
     </row>
     <row r="168" spans="3:29">
-      <c r="C168" s="30"/>
+      <c r="C168" s="33"/>
       <c r="D168" s="1"/>
       <c r="E168" s="5">
         <v>0.67206478118896396</v>
@@ -3319,11 +3343,11 @@
       </c>
     </row>
     <row r="169" spans="3:29">
-      <c r="C169" s="30"/>
+      <c r="C169" s="33"/>
       <c r="D169" s="1"/>
     </row>
     <row r="170" spans="3:29">
-      <c r="C170" s="30"/>
+      <c r="C170" s="33"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1" t="s">
         <v>1</v>
@@ -3348,7 +3372,7 @@
       </c>
     </row>
     <row r="171" spans="3:29">
-      <c r="C171" s="30"/>
+      <c r="C171" s="33"/>
       <c r="D171" s="1"/>
       <c r="E171" s="10">
         <f>AVERAGE(E166:E168)</f>
@@ -3503,9 +3527,9 @@
       </c>
     </row>
     <row r="188" spans="3:9">
-      <c r="E188" s="28"/>
-      <c r="F188" s="28"/>
-      <c r="G188" s="28"/>
+      <c r="E188" s="31"/>
+      <c r="F188" s="31"/>
+      <c r="G188" s="31"/>
     </row>
     <row r="189" spans="3:9">
       <c r="E189" s="1"/>
@@ -3608,11 +3632,11 @@
       </c>
     </row>
     <row r="203" spans="3:9">
-      <c r="E203" s="28" t="s">
+      <c r="E203" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F203" s="28"/>
-      <c r="G203" s="28"/>
+      <c r="F203" s="31"/>
+      <c r="G203" s="31"/>
     </row>
     <row r="204" spans="3:9">
       <c r="E204" s="1" t="s">
@@ -3626,14 +3650,14 @@
       </c>
     </row>
     <row r="205" spans="3:9">
-      <c r="C205" s="29" t="s">
+      <c r="C205" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D205" s="1">
         <v>0</v>
       </c>
       <c r="E205" s="10"/>
-      <c r="F205" s="32">
+      <c r="F205" s="29">
         <v>0.54898785425101204</v>
       </c>
       <c r="G205" s="12">
@@ -3644,12 +3668,12 @@
       </c>
     </row>
     <row r="206" spans="3:9">
-      <c r="C206" s="30"/>
+      <c r="C206" s="33"/>
       <c r="D206" s="1">
         <v>1</v>
       </c>
       <c r="E206" s="10"/>
-      <c r="F206" s="33" t="s">
+      <c r="F206" s="30" t="s">
         <v>210</v>
       </c>
       <c r="G206" s="10" t="s">
@@ -3660,7 +3684,7 @@
       </c>
     </row>
     <row r="207" spans="3:9">
-      <c r="C207" s="30"/>
+      <c r="C207" s="33"/>
       <c r="D207" s="1">
         <v>2</v>
       </c>
@@ -3676,13 +3700,13 @@
       </c>
     </row>
     <row r="208" spans="3:9">
-      <c r="C208" s="30"/>
+      <c r="C208" s="33"/>
       <c r="D208" s="1">
         <v>3</v>
       </c>
       <c r="E208" s="10"/>
       <c r="F208" s="10"/>
-      <c r="G208" s="33" t="s">
+      <c r="G208" s="30" t="s">
         <v>210</v>
       </c>
       <c r="I208" s="16" t="s">
@@ -3690,7 +3714,7 @@
       </c>
     </row>
     <row r="209" spans="3:9">
-      <c r="C209" s="30"/>
+      <c r="C209" s="33"/>
       <c r="D209" s="1">
         <v>4</v>
       </c>
@@ -3698,7 +3722,7 @@
       <c r="F209" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G209" s="33" t="s">
+      <c r="G209" s="30" t="s">
         <v>160</v>
       </c>
       <c r="I209" s="16" t="s">
@@ -3706,7 +3730,7 @@
       </c>
     </row>
     <row r="210" spans="3:9">
-      <c r="C210" s="30"/>
+      <c r="C210" s="33"/>
       <c r="D210" s="1">
         <v>5</v>
       </c>
@@ -3721,13 +3745,200 @@
         <v>28</v>
       </c>
     </row>
+    <row r="213" spans="3:9" ht="15.75" thickBot="1">
+      <c r="F213" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="3:9">
+      <c r="E214">
+        <v>0.54251009225845304</v>
+      </c>
+      <c r="F214">
+        <v>0.52631580829620295</v>
+      </c>
+    </row>
+    <row r="215" spans="3:9">
+      <c r="E215">
+        <v>0.53441298007964999</v>
+      </c>
+      <c r="F215">
+        <v>0.53441298007964999</v>
+      </c>
+    </row>
+    <row r="216" spans="3:9">
+      <c r="E216" s="37">
+        <v>0.48582994937896701</v>
+      </c>
+      <c r="F216" s="37">
+        <v>0.48178136348724299</v>
+      </c>
+      <c r="G216" s="28"/>
+    </row>
+    <row r="217" spans="3:9">
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="1"/>
+    </row>
+    <row r="218" spans="3:9">
+      <c r="C218" s="35"/>
+      <c r="D218" s="1"/>
+      <c r="E218" s="10"/>
+      <c r="F218" s="29"/>
+      <c r="G218" s="12"/>
+      <c r="I218" s="16"/>
+    </row>
+    <row r="219" spans="3:9">
+      <c r="C219" s="36"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="10"/>
+      <c r="F219" s="30"/>
+      <c r="G219" s="10"/>
+      <c r="I219" s="16"/>
+    </row>
+    <row r="220" spans="3:9">
+      <c r="D220" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G220" s="15"/>
+      <c r="I220" s="16"/>
+    </row>
+    <row r="221" spans="3:9">
+      <c r="C221" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D221" s="10"/>
+      <c r="E221" s="10">
+        <f>AVERAGE(E214:E216)</f>
+        <v>0.52091767390568999</v>
+      </c>
+      <c r="F221" s="10">
+        <f>AVERAGE(F214:F216)</f>
+        <v>0.51417005062103194</v>
+      </c>
+      <c r="G221" s="30"/>
+      <c r="I221" s="16"/>
+    </row>
+    <row r="222" spans="3:9">
+      <c r="C222" s="36"/>
+      <c r="D222" s="1"/>
+      <c r="E222" s="15"/>
+      <c r="F222" s="10"/>
+      <c r="G222" s="30"/>
+      <c r="I222" s="16"/>
+    </row>
+    <row r="223" spans="3:9">
+      <c r="C223" s="36"/>
+      <c r="D223" s="1"/>
+      <c r="E223" s="15"/>
+      <c r="F223" s="5"/>
+      <c r="G223" s="5"/>
+      <c r="I223" s="16"/>
+    </row>
+    <row r="226" spans="3:9" ht="15.75" thickBot="1">
+      <c r="F226" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="227" spans="3:9">
+      <c r="E227">
+        <v>0.51417005062103205</v>
+      </c>
+      <c r="F227">
+        <v>0.53036439418792702</v>
+      </c>
+    </row>
+    <row r="228" spans="3:9">
+      <c r="E228">
+        <v>0.51821863651275601</v>
+      </c>
+      <c r="F228">
+        <v>0.55060726404189997</v>
+      </c>
+    </row>
+    <row r="229" spans="3:9">
+      <c r="E229" s="37">
+        <v>0.546558678150177</v>
+      </c>
+      <c r="F229" s="37">
+        <v>0.56275302171707098</v>
+      </c>
+      <c r="G229" s="28"/>
+    </row>
+    <row r="230" spans="3:9">
+      <c r="E230" s="1"/>
+      <c r="F230" s="1"/>
+      <c r="G230" s="1"/>
+    </row>
+    <row r="231" spans="3:9">
+      <c r="C231" s="35"/>
+      <c r="D231" s="1"/>
+      <c r="E231" s="10"/>
+      <c r="F231" s="29"/>
+      <c r="G231" s="12"/>
+      <c r="I231" s="16"/>
+    </row>
+    <row r="232" spans="3:9">
+      <c r="C232" s="36"/>
+      <c r="D232" s="1"/>
+      <c r="E232" s="10"/>
+      <c r="F232" s="30"/>
+      <c r="G232" s="10"/>
+      <c r="I232" s="16"/>
+    </row>
+    <row r="233" spans="3:9">
+      <c r="C233" s="36"/>
+      <c r="D233" s="1"/>
+      <c r="E233" s="15"/>
+      <c r="F233" s="15"/>
+      <c r="G233" s="15"/>
+      <c r="I233" s="16"/>
+    </row>
+    <row r="234" spans="3:9">
+      <c r="D234" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G234" s="30"/>
+      <c r="I234" s="16"/>
+    </row>
+    <row r="235" spans="3:9">
+      <c r="C235" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D235" s="10"/>
+      <c r="E235" s="10">
+        <f>AVERAGE(E227:E229)</f>
+        <v>0.52631578842798843</v>
+      </c>
+      <c r="F235" s="10">
+        <f>AVERAGE(F227:F229)</f>
+        <v>0.54790822664896599</v>
+      </c>
+      <c r="G235" s="30"/>
+      <c r="I235" s="16"/>
+    </row>
+    <row r="236" spans="3:9">
+      <c r="C236" s="36"/>
+      <c r="D236" s="1"/>
+      <c r="E236" s="15"/>
+      <c r="F236" s="5"/>
+      <c r="G236" s="5"/>
+      <c r="I236" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E203:G203"/>
-    <mergeCell ref="C205:C210"/>
-    <mergeCell ref="E164:G164"/>
-    <mergeCell ref="C166:C171"/>
-    <mergeCell ref="E188:G188"/>
     <mergeCell ref="E143:G143"/>
     <mergeCell ref="C145:C150"/>
     <mergeCell ref="C2:E2"/>
@@ -3740,6 +3951,11 @@
     <mergeCell ref="C82:C87"/>
     <mergeCell ref="E101:G101"/>
     <mergeCell ref="C103:C108"/>
+    <mergeCell ref="E203:G203"/>
+    <mergeCell ref="C205:C210"/>
+    <mergeCell ref="E164:G164"/>
+    <mergeCell ref="C166:C171"/>
+    <mergeCell ref="E188:G188"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Change models config file and calculate average accuracy for algorithms results
</commit_message>
<xml_diff>
--- a/algorithms_results.xlsx
+++ b/algorithms_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Studia\mgr\praca_magisterska\auth-smile-classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8374F4-5D12-4D2A-BDE3-39A1397EAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162E5F50-67E8-42F9-B4E7-2198815432B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-144" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="238">
   <si>
     <t>scaled</t>
   </si>
@@ -676,24 +676,106 @@
   </si>
   <si>
     <t>BRWI 3</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>ŚREDNIE</t>
+  </si>
+  <si>
+    <t>kaciki</t>
+  </si>
+  <si>
+    <t>odl od nosa</t>
+  </si>
+  <si>
+    <t>kat</t>
+  </si>
+  <si>
+    <t>odl od siebie</t>
+  </si>
+  <si>
+    <t>twarz 2</t>
+  </si>
+  <si>
+    <t>twarz 3</t>
+  </si>
+  <si>
+    <t>metoda do danych</t>
+  </si>
+  <si>
+    <t>algorytm</t>
+  </si>
+  <si>
+    <t>kNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">las losowy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">twarz </t>
+  </si>
+  <si>
+    <t>ale bez twarzy (8 wartości)</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>kąciki</t>
+  </si>
+  <si>
+    <t>kąciki - odl od nosa</t>
+  </si>
+  <si>
+    <t>kąt</t>
+  </si>
+  <si>
+    <t>kąciki - odl od siebie</t>
+  </si>
+  <si>
+    <t>twarz</t>
+  </si>
+  <si>
+    <t>brwi</t>
+  </si>
+  <si>
+    <t>bez domyslnej LSTM i BOSSVS</t>
+  </si>
+  <si>
+    <t>bez BOSSVS</t>
+  </si>
+  <si>
+    <t>tylko domysln.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -832,7 +914,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -858,59 +940,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -919,13 +1080,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
@@ -1207,28 +1376,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AL236"/>
+  <dimension ref="A2:AL284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="F223" sqref="F223"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="H284" sqref="H284"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -1242,7 +1412,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -1262,7 +1432,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="33"/>
+      <c r="A5" s="35"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -1280,7 +1450,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="33"/>
+      <c r="A6" s="35"/>
       <c r="B6">
         <v>2</v>
       </c>
@@ -1298,7 +1468,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="33"/>
+      <c r="A7" s="35"/>
       <c r="B7">
         <v>3</v>
       </c>
@@ -1316,7 +1486,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="33"/>
+      <c r="A8" s="35"/>
       <c r="B8">
         <v>4</v>
       </c>
@@ -1334,7 +1504,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="33"/>
+      <c r="A9" s="35"/>
       <c r="B9">
         <v>5</v>
       </c>
@@ -1422,17 +1592,17 @@
       </c>
     </row>
     <row r="23" spans="3:25">
-      <c r="C23" s="9">
-        <f>AVERAGE(C25:C29)*100</f>
-        <v>69.311741590499835</v>
-      </c>
-      <c r="D23" s="9">
-        <f>AVERAGE(D25:D29)*100</f>
-        <v>74.574898481368962</v>
-      </c>
-      <c r="E23" s="9">
-        <f>AVERAGE(E25:E29)*100</f>
-        <v>76.275304555892887</v>
+      <c r="C23" s="8">
+        <f>AVERAGE(C25:C29)</f>
+        <v>0.69311741590499831</v>
+      </c>
+      <c r="D23" s="8">
+        <f>AVERAGE(D25:D29)</f>
+        <v>0.74574898481368956</v>
+      </c>
+      <c r="E23" s="8">
+        <f>AVERAGE(E25:E29)</f>
+        <v>0.76275304555892887</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>2</v>
@@ -1820,17 +1990,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="3:25" ht="15.75" thickBot="1">
-      <c r="F58" s="13" t="s">
+    <row r="58" spans="3:25" ht="15" thickBot="1">
+      <c r="F58" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="59" spans="3:25">
-      <c r="E59" s="31" t="s">
+      <c r="E59" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
     </row>
     <row r="60" spans="3:25">
       <c r="E60" s="1" t="s">
@@ -1844,22 +2014,22 @@
       </c>
     </row>
     <row r="61" spans="3:25">
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="9">
         <v>0.58056680161943297</v>
       </c>
       <c r="F61" s="8">
         <v>0.67287449392712495</v>
       </c>
-      <c r="G61" s="12">
+      <c r="G61" s="11">
         <v>0.68016194331983804</v>
       </c>
-      <c r="I61" s="16" t="s">
+      <c r="I61" s="15" t="s">
         <v>23</v>
       </c>
       <c r="M61" t="s">
@@ -1867,20 +2037,20 @@
       </c>
     </row>
     <row r="62" spans="3:25">
-      <c r="C62" s="32"/>
+      <c r="C62" s="34"/>
       <c r="D62" s="1">
         <v>1</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62" s="9">
         <v>0.54170040485829896</v>
       </c>
       <c r="F62" s="8">
         <v>0.668016194331983</v>
       </c>
-      <c r="G62" s="10">
+      <c r="G62" s="9">
         <v>0.59676113360323801</v>
       </c>
-      <c r="I62" s="16" t="s">
+      <c r="I62" s="15" t="s">
         <v>24</v>
       </c>
       <c r="M62" t="s">
@@ -1888,38 +2058,38 @@
       </c>
     </row>
     <row r="63" spans="3:25">
-      <c r="C63" s="32"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="1">
         <v>2</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="10">
         <v>0.67611336032388603</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="10">
         <v>0.72793522267206401</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="13">
         <v>0.75748987854251004</v>
       </c>
-      <c r="I63" s="16" t="s">
+      <c r="I63" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="3:25">
-      <c r="C64" s="32"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="1">
         <v>3</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="9">
         <v>0.60242914979757001</v>
       </c>
-      <c r="F64" s="10">
+      <c r="F64" s="9">
         <v>0.65546558704453395</v>
       </c>
       <c r="G64" s="8">
         <v>0.70526315789473604</v>
       </c>
-      <c r="I64" s="16" t="s">
+      <c r="I64" s="15" t="s">
         <v>26</v>
       </c>
       <c r="M64" t="s">
@@ -1927,43 +2097,43 @@
       </c>
     </row>
     <row r="65" spans="3:9">
-      <c r="C65" s="32"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="1">
         <v>4</v>
       </c>
       <c r="E65" s="8">
         <v>0.60769230769230698</v>
       </c>
-      <c r="F65" s="10">
+      <c r="F65" s="9">
         <v>0.64453441295546499</v>
       </c>
       <c r="G65" s="8">
         <v>0.68421052631578905</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="I65" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="66" spans="3:9">
-      <c r="C66" s="32"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="1">
         <v>5</v>
       </c>
       <c r="E66" s="8">
         <v>0.62793522267206403</v>
       </c>
-      <c r="F66" s="10">
+      <c r="F66" s="9">
         <v>0.65546558704453395</v>
       </c>
-      <c r="G66" s="10">
+      <c r="G66" s="9">
         <v>0.65789473684210498</v>
       </c>
-      <c r="I66" s="16" t="s">
+      <c r="I66" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="3:9" ht="15.75" thickBot="1">
-      <c r="F70" s="13" t="s">
+    <row r="70" spans="3:9" ht="15" thickBot="1">
+      <c r="F70" s="12" t="s">
         <v>99</v>
       </c>
       <c r="G70" t="s">
@@ -2040,25 +2210,25 @@
       <c r="C78" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="9">
         <f>AVERAGE(D71:D75)</f>
         <v>0.52550606727600058</v>
       </c>
-      <c r="E78" s="10">
+      <c r="E78" s="9">
         <f>AVERAGE(E71:E75)</f>
         <v>0.66639676094055145</v>
       </c>
-      <c r="F78" s="10">
+      <c r="F78" s="9">
         <f>AVERAGE(F71:F75)</f>
         <v>0.66234817504882759</v>
       </c>
     </row>
     <row r="80" spans="3:9">
-      <c r="E80" s="31" t="s">
+      <c r="E80" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
     </row>
     <row r="81" spans="3:33">
       <c r="E81" s="1" t="s">
@@ -2072,103 +2242,103 @@
       </c>
     </row>
     <row r="82" spans="3:33">
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E82" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F82" s="25">
+      <c r="F82" s="24">
         <v>0.56356275303643699</v>
       </c>
-      <c r="G82" s="24">
+      <c r="G82" s="23">
         <v>0.58744939271255003</v>
       </c>
-      <c r="I82" s="16" t="s">
+      <c r="I82" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="83" spans="3:33">
-      <c r="C83" s="33"/>
+      <c r="C83" s="35"/>
       <c r="D83" s="1">
         <v>1</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F83" s="25">
+      <c r="F83" s="24">
         <v>0.50404858299595101</v>
       </c>
       <c r="G83" s="5">
         <v>0.52307692307692299</v>
       </c>
-      <c r="I83" s="16" t="s">
+      <c r="I83" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="84" spans="3:33">
-      <c r="C84" s="33"/>
+      <c r="C84" s="35"/>
       <c r="D84" s="1">
         <v>2</v>
       </c>
-      <c r="E84" s="15" t="s">
+      <c r="E84" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F84" s="25">
+      <c r="F84" s="24">
         <v>0.66437246963562702</v>
       </c>
-      <c r="G84" s="25">
+      <c r="G84" s="24">
         <v>0.65546558704453395</v>
       </c>
-      <c r="I84" s="16" t="s">
+      <c r="I84" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="3:33">
-      <c r="C85" s="33"/>
+      <c r="C85" s="35"/>
       <c r="D85" s="1">
         <v>3</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E85" s="9" t="s">
         <v>105</v>
       </c>
       <c r="F85" s="5">
         <v>0.58461538461538398</v>
       </c>
-      <c r="G85" s="25">
+      <c r="G85" s="24">
         <v>0.60485829959514104</v>
       </c>
-      <c r="I85" s="16" t="s">
+      <c r="I85" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="86" spans="3:33">
-      <c r="C86" s="33"/>
+      <c r="C86" s="35"/>
       <c r="D86" s="1">
         <v>4</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="E86" s="14" t="s">
         <v>103</v>
       </c>
       <c r="F86" s="5">
         <v>0.63441295546558696</v>
       </c>
-      <c r="G86" s="25">
+      <c r="G86" s="24">
         <v>0.61417004048582902</v>
       </c>
-      <c r="I86" s="16" t="s">
+      <c r="I86" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="87" spans="3:33">
-      <c r="C87" s="33"/>
+      <c r="C87" s="35"/>
       <c r="D87" s="1">
         <v>5</v>
       </c>
-      <c r="E87" s="15" t="s">
+      <c r="E87" s="14" t="s">
         <v>104</v>
       </c>
       <c r="F87" s="5">
@@ -2177,12 +2347,12 @@
       <c r="G87" s="5">
         <v>0.540485829959514</v>
       </c>
-      <c r="I87" s="16" t="s">
+      <c r="I87" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="3:33" ht="15.75" thickBot="1">
-      <c r="F91" s="13" t="s">
+    <row r="91" spans="3:33" ht="15" thickBot="1">
+      <c r="F91" s="12" t="s">
         <v>107</v>
       </c>
       <c r="G91" t="s">
@@ -2324,15 +2494,15 @@
       <c r="C99" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D99" s="10" t="e">
+      <c r="D99" s="9" t="e">
         <f>AVERAGE(D92:D96)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99" s="9">
         <f>AVERAGE(E92:E96)</f>
         <v>0.73279350996017367</v>
       </c>
-      <c r="F99" s="10">
+      <c r="F99" s="9">
         <f>AVERAGE(F92:F96)</f>
         <v>0.76518217325210514</v>
       </c>
@@ -2376,11 +2546,11 @@
       </c>
     </row>
     <row r="101" spans="3:33">
-      <c r="E101" s="31" t="s">
+      <c r="E101" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F101" s="31"/>
-      <c r="G101" s="31"/>
+      <c r="F101" s="33"/>
+      <c r="G101" s="33"/>
       <c r="H101" t="s">
         <v>113</v>
       </c>
@@ -2412,105 +2582,105 @@
       </c>
     </row>
     <row r="103" spans="3:33">
-      <c r="C103" s="32" t="s">
+      <c r="C103" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
       </c>
-      <c r="E103" s="10"/>
-      <c r="F103" s="23">
+      <c r="E103" s="9"/>
+      <c r="F103" s="22">
         <v>0.68623481781376505</v>
       </c>
-      <c r="G103" s="24">
+      <c r="G103" s="23">
         <v>0.67004048582995901</v>
       </c>
-      <c r="I103" s="16" t="s">
+      <c r="I103" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="104" spans="3:33">
-      <c r="C104" s="33"/>
+      <c r="C104" s="35"/>
       <c r="D104" s="1">
         <v>1</v>
       </c>
-      <c r="E104" s="10"/>
-      <c r="F104" s="25">
+      <c r="E104" s="9"/>
+      <c r="F104" s="24">
         <v>0.54008097165991897</v>
       </c>
       <c r="G104" s="5">
         <v>0.61740890688259098</v>
       </c>
-      <c r="I104" s="16" t="s">
+      <c r="I104" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="105" spans="3:33">
-      <c r="C105" s="33"/>
+      <c r="C105" s="35"/>
       <c r="D105" s="1">
         <v>2</v>
       </c>
-      <c r="E105" s="15"/>
-      <c r="F105" s="25">
+      <c r="E105" s="14"/>
+      <c r="F105" s="24">
         <v>0.76194331983805597</v>
       </c>
-      <c r="G105" s="25">
+      <c r="G105" s="24">
         <v>0.76315789473684204</v>
       </c>
-      <c r="I105" s="16" t="s">
+      <c r="I105" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="106" spans="3:33">
-      <c r="C106" s="33"/>
+      <c r="C106" s="35"/>
       <c r="D106" s="1">
         <v>3</v>
       </c>
-      <c r="E106" s="10"/>
+      <c r="E106" s="9"/>
       <c r="F106" s="5">
         <v>0.68906882591093099</v>
       </c>
-      <c r="G106" s="25">
+      <c r="G106" s="24">
         <v>0.70202429149797496</v>
       </c>
-      <c r="I106" s="16" t="s">
+      <c r="I106" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="107" spans="3:33">
-      <c r="C107" s="33"/>
+      <c r="C107" s="35"/>
       <c r="D107" s="1">
         <v>4</v>
       </c>
-      <c r="E107" s="15"/>
+      <c r="E107" s="14"/>
       <c r="F107" s="5">
         <v>0.708502024291498</v>
       </c>
-      <c r="G107" s="25">
+      <c r="G107" s="24">
         <v>0.72267206477732704</v>
       </c>
-      <c r="I107" s="16" t="s">
+      <c r="I107" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="108" spans="3:33">
-      <c r="C108" s="33"/>
+      <c r="C108" s="35"/>
       <c r="D108" s="1">
         <v>5</v>
       </c>
-      <c r="E108" s="15"/>
+      <c r="E108" s="14"/>
       <c r="F108" s="5">
         <v>0.63643724696356196</v>
       </c>
       <c r="G108" s="5">
         <v>0.72550607287449398</v>
       </c>
-      <c r="I108" s="16" t="s">
+      <c r="I108" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="3:33" ht="15.75" thickBot="1">
-      <c r="F112" s="13" t="s">
+    <row r="112" spans="3:33" ht="15" thickBot="1">
+      <c r="F112" s="12" t="s">
         <v>108</v>
       </c>
       <c r="G112" t="s">
@@ -2664,12 +2834,12 @@
       <c r="C120" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10">
+      <c r="D120" s="9"/>
+      <c r="E120" s="9">
         <f>AVERAGE(E113:E117)</f>
         <v>0.72874493598937939</v>
       </c>
-      <c r="F120" s="10">
+      <c r="F120" s="9">
         <f>AVERAGE(F113:F117)</f>
         <v>0.760323894023895</v>
       </c>
@@ -2719,11 +2889,11 @@
       </c>
     </row>
     <row r="122" spans="3:38">
-      <c r="E122" s="31" t="s">
+      <c r="E122" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F122" s="31"/>
-      <c r="G122" s="31"/>
+      <c r="F122" s="33"/>
+      <c r="G122" s="33"/>
       <c r="H122" t="s">
         <v>133</v>
       </c>
@@ -2758,105 +2928,105 @@
       </c>
     </row>
     <row r="124" spans="3:38">
-      <c r="C124" s="32" t="s">
+      <c r="C124" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="1">
         <v>0</v>
       </c>
-      <c r="E124" s="10"/>
-      <c r="F124" s="17">
+      <c r="E124" s="9"/>
+      <c r="F124" s="16">
         <v>0.65101214574898703</v>
       </c>
-      <c r="G124" s="12">
+      <c r="G124" s="11">
         <v>0.66315789473684195</v>
       </c>
-      <c r="I124" s="16" t="s">
+      <c r="I124" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="125" spans="3:38">
-      <c r="C125" s="33"/>
+      <c r="C125" s="35"/>
       <c r="D125" s="1">
         <v>1</v>
       </c>
-      <c r="E125" s="10"/>
-      <c r="F125" s="15">
+      <c r="E125" s="9"/>
+      <c r="F125" s="14">
         <v>0.50931174089068798</v>
       </c>
-      <c r="G125" s="10">
+      <c r="G125" s="9">
         <v>0.54089068825910902</v>
       </c>
-      <c r="I125" s="16" t="s">
+      <c r="I125" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="3:38">
-      <c r="C126" s="33"/>
+      <c r="C126" s="35"/>
       <c r="D126" s="1">
         <v>2</v>
       </c>
-      <c r="E126" s="15"/>
-      <c r="F126" s="15">
+      <c r="E126" s="14"/>
+      <c r="F126" s="14">
         <v>0.72550607287449398</v>
       </c>
-      <c r="G126" s="15">
+      <c r="G126" s="14">
         <v>0.72186234817813699</v>
       </c>
-      <c r="I126" s="16" t="s">
+      <c r="I126" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="127" spans="3:38">
-      <c r="C127" s="33"/>
+      <c r="C127" s="35"/>
       <c r="D127" s="1">
         <v>3</v>
       </c>
-      <c r="E127" s="10"/>
-      <c r="F127" s="10">
+      <c r="E127" s="9"/>
+      <c r="F127" s="9">
         <v>0.675708502024291</v>
       </c>
-      <c r="G127" s="15">
+      <c r="G127" s="14">
         <v>0.67489878542510096</v>
       </c>
-      <c r="I127" s="16" t="s">
+      <c r="I127" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="128" spans="3:38">
-      <c r="C128" s="33"/>
+      <c r="C128" s="35"/>
       <c r="D128" s="1">
         <v>4</v>
       </c>
-      <c r="E128" s="15"/>
-      <c r="F128" s="10">
+      <c r="E128" s="14"/>
+      <c r="F128" s="9">
         <v>0.7</v>
       </c>
-      <c r="G128" s="15">
+      <c r="G128" s="14">
         <v>0.72550607287449398</v>
       </c>
-      <c r="I128" s="16" t="s">
+      <c r="I128" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="129" spans="3:22">
-      <c r="C129" s="33"/>
+      <c r="C129" s="35"/>
       <c r="D129" s="1">
         <v>5</v>
       </c>
-      <c r="E129" s="15"/>
-      <c r="F129" s="10">
+      <c r="E129" s="14"/>
+      <c r="F129" s="9">
         <v>0.62591093117408902</v>
       </c>
-      <c r="G129" s="10">
+      <c r="G129" s="9">
         <v>0.69068825910931098</v>
       </c>
-      <c r="I129" s="16" t="s">
+      <c r="I129" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="3:22" ht="15.75" thickBot="1">
-      <c r="F133" s="13" t="s">
+    <row r="133" spans="3:22" ht="15" thickBot="1">
+      <c r="F133" s="12" t="s">
         <v>149</v>
       </c>
       <c r="G133" t="s">
@@ -2864,10 +3034,10 @@
       </c>
     </row>
     <row r="134" spans="3:22">
-      <c r="E134" s="10">
+      <c r="E134" s="9">
         <v>0.57085019350051802</v>
       </c>
-      <c r="F134" s="10">
+      <c r="F134" s="9">
         <v>0.546558678150177</v>
       </c>
       <c r="H134" s="1"/>
@@ -2879,10 +3049,10 @@
       </c>
     </row>
     <row r="135" spans="3:22">
-      <c r="E135" s="10">
+      <c r="E135" s="9">
         <v>0.53036439418792702</v>
       </c>
-      <c r="F135" s="10">
+      <c r="F135" s="9">
         <v>0.55465584993362405</v>
       </c>
       <c r="L135">
@@ -2896,10 +3066,10 @@
       </c>
     </row>
     <row r="136" spans="3:22">
-      <c r="E136" s="10">
+      <c r="E136" s="9">
         <v>0.48987853527068997</v>
       </c>
-      <c r="F136" s="10">
+      <c r="F136" s="9">
         <v>0.53036439418792702</v>
       </c>
       <c r="L136" t="s">
@@ -2956,12 +3126,12 @@
       <c r="C141" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D141" s="10"/>
-      <c r="E141" s="10">
+      <c r="D141" s="9"/>
+      <c r="E141" s="9">
         <f>AVERAGE(E134:E136)</f>
         <v>0.53036437431971173</v>
       </c>
-      <c r="F141" s="10">
+      <c r="F141" s="9">
         <f>AVERAGE(F134:F136)</f>
         <v>0.54385964075724269</v>
       </c>
@@ -2987,11 +3157,11 @@
       </c>
     </row>
     <row r="143" spans="3:22">
-      <c r="E143" s="31" t="s">
+      <c r="E143" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F143" s="31"/>
-      <c r="G143" s="31"/>
+      <c r="F143" s="33"/>
+      <c r="G143" s="33"/>
       <c r="L143" t="s">
         <v>154</v>
       </c>
@@ -3014,108 +3184,108 @@
       </c>
     </row>
     <row r="145" spans="3:24">
-      <c r="C145" s="32" t="s">
+      <c r="C145" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="1">
         <v>0</v>
       </c>
-      <c r="E145" s="10"/>
-      <c r="F145" s="29">
+      <c r="E145" s="9"/>
+      <c r="F145" s="28">
         <v>0.70526315789473604</v>
       </c>
-      <c r="G145" s="12">
+      <c r="G145" s="11">
         <v>0.69716599190283401</v>
       </c>
-      <c r="I145" s="16" t="s">
+      <c r="I145" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="146" spans="3:24">
-      <c r="C146" s="33"/>
+      <c r="C146" s="35"/>
       <c r="D146" s="1">
         <v>1</v>
       </c>
-      <c r="E146" s="10"/>
-      <c r="F146" s="18" t="s">
+      <c r="E146" s="9"/>
+      <c r="F146" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G146" s="10" t="s">
+      <c r="G146" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I146" s="16" t="s">
+      <c r="I146" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="147" spans="3:24">
-      <c r="C147" s="33"/>
+      <c r="C147" s="35"/>
       <c r="D147" s="1">
         <v>2</v>
       </c>
-      <c r="E147" s="15"/>
-      <c r="F147" s="15">
+      <c r="E147" s="14"/>
+      <c r="F147" s="14">
         <v>0.72024291497975701</v>
       </c>
-      <c r="G147" s="15">
+      <c r="G147" s="14">
         <v>0.70809716599190198</v>
       </c>
-      <c r="I147" s="16" t="s">
+      <c r="I147" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="148" spans="3:24">
-      <c r="C148" s="33"/>
+      <c r="C148" s="35"/>
       <c r="D148" s="1">
         <v>3</v>
       </c>
-      <c r="E148" s="10"/>
-      <c r="F148" s="10" t="s">
+      <c r="E148" s="9"/>
+      <c r="F148" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G148" s="19" t="s">
+      <c r="G148" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="I148" s="16" t="s">
+      <c r="I148" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="149" spans="3:24">
-      <c r="C149" s="33"/>
+      <c r="C149" s="35"/>
       <c r="D149" s="1">
         <v>4</v>
       </c>
-      <c r="E149" s="15"/>
-      <c r="F149" s="10" t="s">
+      <c r="E149" s="14"/>
+      <c r="F149" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G149" s="18" t="s">
+      <c r="G149" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I149" s="16" t="s">
+      <c r="I149" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="150" spans="3:24">
-      <c r="C150" s="33"/>
+      <c r="C150" s="35"/>
       <c r="D150" s="1">
         <v>5</v>
       </c>
-      <c r="E150" s="15"/>
+      <c r="E150" s="14"/>
       <c r="F150" s="5">
         <v>0.65951417004048496</v>
       </c>
       <c r="G150" s="5">
         <v>0.53886639676113302</v>
       </c>
-      <c r="I150" s="16" t="s">
+      <c r="I150" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="3:24" ht="15.75" thickBot="1">
-      <c r="F153" s="13" t="s">
+    <row r="153" spans="3:24" ht="15" thickBot="1">
+      <c r="F153" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="I153" s="16" t="s">
+      <c r="I153" s="15" t="s">
         <v>1</v>
       </c>
       <c r="S153" s="1" t="s">
@@ -3227,12 +3397,12 @@
       <c r="C161" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D161" s="10"/>
-      <c r="E161" s="10">
+      <c r="D161" s="9"/>
+      <c r="E161" s="9">
         <f>AVERAGE(E154:E156)</f>
         <v>0.63832658529281572</v>
       </c>
-      <c r="F161" s="10">
+      <c r="F161" s="9">
         <f>AVERAGE(F154:F156)</f>
         <v>0.67206476132074933</v>
       </c>
@@ -3264,20 +3434,20 @@
       </c>
     </row>
     <row r="164" spans="3:29">
-      <c r="E164" s="31"/>
-      <c r="F164" s="31"/>
-      <c r="G164" s="31"/>
-    </row>
-    <row r="165" spans="3:29" ht="15.75" thickBot="1">
+      <c r="E164" s="33"/>
+      <c r="F164" s="33"/>
+      <c r="G164" s="33"/>
+    </row>
+    <row r="165" spans="3:29" ht="15" thickBot="1">
       <c r="E165" t="s">
         <v>187</v>
       </c>
-      <c r="F165" s="13" t="s">
+      <c r="F165" s="12" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="166" spans="3:29">
-      <c r="C166" s="32"/>
+      <c r="C166" s="34"/>
       <c r="D166" s="1"/>
       <c r="E166" s="5">
         <v>0.65587043762206998</v>
@@ -3293,7 +3463,7 @@
       </c>
     </row>
     <row r="167" spans="3:29">
-      <c r="C167" s="33"/>
+      <c r="C167" s="35"/>
       <c r="D167" s="1"/>
       <c r="E167" s="5">
         <v>0.70445346832275302</v>
@@ -3318,7 +3488,7 @@
       </c>
     </row>
     <row r="168" spans="3:29">
-      <c r="C168" s="33"/>
+      <c r="C168" s="35"/>
       <c r="D168" s="1"/>
       <c r="E168" s="5">
         <v>0.67206478118896396</v>
@@ -3343,11 +3513,11 @@
       </c>
     </row>
     <row r="169" spans="3:29">
-      <c r="C169" s="33"/>
+      <c r="C169" s="35"/>
       <c r="D169" s="1"/>
     </row>
     <row r="170" spans="3:29">
-      <c r="C170" s="33"/>
+      <c r="C170" s="35"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1" t="s">
         <v>1</v>
@@ -3372,13 +3542,13 @@
       </c>
     </row>
     <row r="171" spans="3:29">
-      <c r="C171" s="33"/>
+      <c r="C171" s="35"/>
       <c r="D171" s="1"/>
-      <c r="E171" s="10">
+      <c r="E171" s="9">
         <f>AVERAGE(E166:E168)</f>
         <v>0.67746289571126228</v>
       </c>
-      <c r="F171" s="10">
+      <c r="F171" s="9">
         <f>AVERAGE(F166:F168)</f>
         <v>0.64102564255396466</v>
       </c>
@@ -3455,22 +3625,22 @@
       </c>
     </row>
     <row r="181" spans="3:9">
-      <c r="C181" s="22" t="s">
+      <c r="C181" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D181" s="21">
+      <c r="D181" s="20">
         <f>AVERAGE(F61:G61,F82:G82,F103:G103,F124:G124,F145:G145)</f>
         <v>0.65769230769230724</v>
       </c>
-      <c r="E181" s="22">
+      <c r="E181" s="21">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="3:9">
-      <c r="C182" s="16" t="s">
+      <c r="C182" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D182" s="10">
+      <c r="D182" s="9">
         <f>AVERAGE(F62:G62,F83:G83,F104:G104,F125:G125)</f>
         <v>0.56244939271255023</v>
       </c>
@@ -3479,14 +3649,14 @@
       </c>
     </row>
     <row r="183" spans="3:9">
-      <c r="C183" s="22" t="s">
+      <c r="C183" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D183" s="21">
+      <c r="D183" s="20">
         <f>AVERAGE(F63:G63,F84:G84,F105:G105,F126:G126,F147:G147)</f>
         <v>0.72060728744939229</v>
       </c>
-      <c r="E183" s="22">
+      <c r="E183" s="21">
         <v>1</v>
       </c>
     </row>
@@ -3494,7 +3664,7 @@
       <c r="C184" t="s">
         <v>26</v>
       </c>
-      <c r="D184" s="10">
+      <c r="D184" s="9">
         <f>AVERAGE(F64:G64,F85:G85,F106:G106,F127:G127)</f>
         <v>0.66148785425101164</v>
       </c>
@@ -3503,22 +3673,22 @@
       </c>
     </row>
     <row r="185" spans="3:9">
-      <c r="C185" s="20" t="s">
+      <c r="C185" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D185" s="21">
+      <c r="D185" s="20">
         <f>AVERAGE(F65:G65,F86:G86,F107:G107,F128:G128)</f>
         <v>0.67925101214574868</v>
       </c>
-      <c r="E185" s="22">
+      <c r="E185" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="186" spans="3:9">
-      <c r="C186" s="16" t="s">
+      <c r="C186" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D186" s="10">
+      <c r="D186" s="9">
         <f t="shared" ref="D186" si="0">AVERAGE(F66:G66,F87:G87,F108:G108,F129:G129,F150:G150)</f>
         <v>0.62935222672064728</v>
       </c>
@@ -3527,9 +3697,9 @@
       </c>
     </row>
     <row r="188" spans="3:9">
-      <c r="E188" s="31"/>
-      <c r="F188" s="31"/>
-      <c r="G188" s="31"/>
+      <c r="E188" s="33"/>
+      <c r="F188" s="33"/>
+      <c r="G188" s="33"/>
     </row>
     <row r="189" spans="3:9">
       <c r="E189" s="1"/>
@@ -3537,28 +3707,28 @@
       <c r="G189" s="1"/>
     </row>
     <row r="190" spans="3:9">
-      <c r="C190" s="26"/>
+      <c r="C190" s="25"/>
       <c r="D190" s="1"/>
-      <c r="E190" s="10"/>
-      <c r="F190" s="17"/>
-      <c r="I190" s="16"/>
+      <c r="E190" s="9"/>
+      <c r="F190" s="16"/>
+      <c r="I190" s="15"/>
     </row>
     <row r="191" spans="3:9">
-      <c r="C191" s="27"/>
+      <c r="C191" s="26"/>
       <c r="D191" s="1"/>
-      <c r="E191" s="10"/>
-      <c r="F191" s="19"/>
-      <c r="I191" s="16"/>
+      <c r="E191" s="9"/>
+      <c r="F191" s="18"/>
+      <c r="I191" s="15"/>
     </row>
     <row r="192" spans="3:9">
-      <c r="C192" s="27"/>
+      <c r="C192" s="26"/>
       <c r="D192" s="1"/>
-      <c r="E192" s="15"/>
-      <c r="F192" s="15"/>
-      <c r="I192" s="16"/>
-    </row>
-    <row r="193" spans="3:9" ht="15.75" thickBot="1">
-      <c r="F193" s="13" t="s">
+      <c r="E192" s="14"/>
+      <c r="F192" s="14"/>
+      <c r="I192" s="15"/>
+    </row>
+    <row r="193" spans="3:9" ht="15" thickBot="1">
+      <c r="F193" s="12" t="s">
         <v>209</v>
       </c>
       <c r="G193" t="s">
@@ -3621,22 +3791,22 @@
       <c r="C201" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D201" s="10"/>
-      <c r="E201" s="10">
+      <c r="D201" s="9"/>
+      <c r="E201" s="9">
         <f>AVERAGE(E194:E198)</f>
         <v>0.53603239059448204</v>
       </c>
-      <c r="F201" s="10">
+      <c r="F201" s="9">
         <f>AVERAGE(F194:F198)</f>
         <v>0.54412955045700018</v>
       </c>
     </row>
     <row r="203" spans="3:9">
-      <c r="E203" s="31" t="s">
+      <c r="E203" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F203" s="31"/>
-      <c r="G203" s="31"/>
+      <c r="F203" s="33"/>
+      <c r="G203" s="33"/>
     </row>
     <row r="204" spans="3:9">
       <c r="E204" s="1" t="s">
@@ -3650,103 +3820,103 @@
       </c>
     </row>
     <row r="205" spans="3:9">
-      <c r="C205" s="32" t="s">
+      <c r="C205" s="34" t="s">
         <v>4</v>
       </c>
       <c r="D205" s="1">
         <v>0</v>
       </c>
-      <c r="E205" s="10"/>
-      <c r="F205" s="29">
+      <c r="E205" s="9"/>
+      <c r="F205" s="28">
         <v>0.54898785425101204</v>
       </c>
-      <c r="G205" s="12">
+      <c r="G205" s="11">
         <v>0.55182186234817798</v>
       </c>
-      <c r="I205" s="16" t="s">
+      <c r="I205" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="206" spans="3:9">
-      <c r="C206" s="33"/>
+      <c r="C206" s="35"/>
       <c r="D206" s="1">
         <v>1</v>
       </c>
-      <c r="E206" s="10"/>
-      <c r="F206" s="30" t="s">
+      <c r="E206" s="9"/>
+      <c r="F206" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G206" s="10" t="s">
+      <c r="G206" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="I206" s="16" t="s">
+      <c r="I206" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="207" spans="3:9">
-      <c r="C207" s="33"/>
+      <c r="C207" s="35"/>
       <c r="D207" s="1">
         <v>2</v>
       </c>
-      <c r="E207" s="15"/>
-      <c r="F207" s="15">
+      <c r="E207" s="14"/>
+      <c r="F207" s="14">
         <v>0.61417004048582902</v>
       </c>
-      <c r="G207" s="15">
+      <c r="G207" s="14">
         <v>0.61740890688259098</v>
       </c>
-      <c r="I207" s="16" t="s">
+      <c r="I207" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="208" spans="3:9">
-      <c r="C208" s="33"/>
+      <c r="C208" s="35"/>
       <c r="D208" s="1">
         <v>3</v>
       </c>
-      <c r="E208" s="10"/>
-      <c r="F208" s="10"/>
-      <c r="G208" s="30" t="s">
+      <c r="E208" s="9"/>
+      <c r="F208" s="9"/>
+      <c r="G208" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="I208" s="16" t="s">
+      <c r="I208" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="209" spans="3:9">
-      <c r="C209" s="33"/>
+      <c r="C209" s="35"/>
       <c r="D209" s="1">
         <v>4</v>
       </c>
-      <c r="E209" s="15"/>
-      <c r="F209" s="10" t="s">
+      <c r="E209" s="14"/>
+      <c r="F209" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G209" s="30" t="s">
+      <c r="G209" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="I209" s="16" t="s">
+      <c r="I209" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="210" spans="3:9">
-      <c r="C210" s="33"/>
+      <c r="C210" s="35"/>
       <c r="D210" s="1">
         <v>5</v>
       </c>
-      <c r="E210" s="15"/>
+      <c r="E210" s="14"/>
       <c r="F210" s="5" t="s">
         <v>210</v>
       </c>
       <c r="G210" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I210" s="16" t="s">
+      <c r="I210" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="213" spans="3:9" ht="15.75" thickBot="1">
-      <c r="F213" s="13" t="s">
+    <row r="213" spans="3:9" ht="15" thickBot="1">
+      <c r="F213" s="12" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3767,13 +3937,13 @@
       </c>
     </row>
     <row r="216" spans="3:9">
-      <c r="E216" s="37">
+      <c r="E216" s="32">
         <v>0.48582994937896701</v>
       </c>
-      <c r="F216" s="37">
+      <c r="F216" s="32">
         <v>0.48178136348724299</v>
       </c>
-      <c r="G216" s="28"/>
+      <c r="G216" s="27"/>
     </row>
     <row r="217" spans="3:9">
       <c r="E217" s="1"/>
@@ -3781,20 +3951,20 @@
       <c r="G217" s="1"/>
     </row>
     <row r="218" spans="3:9">
-      <c r="C218" s="35"/>
+      <c r="C218" s="30"/>
       <c r="D218" s="1"/>
-      <c r="E218" s="10"/>
-      <c r="F218" s="29"/>
-      <c r="G218" s="12"/>
-      <c r="I218" s="16"/>
+      <c r="E218" s="9"/>
+      <c r="F218" s="28"/>
+      <c r="G218" s="11"/>
+      <c r="I218" s="15"/>
     </row>
     <row r="219" spans="3:9">
-      <c r="C219" s="36"/>
+      <c r="C219" s="31"/>
       <c r="D219" s="1"/>
-      <c r="E219" s="10"/>
-      <c r="F219" s="30"/>
-      <c r="G219" s="10"/>
-      <c r="I219" s="16"/>
+      <c r="E219" s="9"/>
+      <c r="F219" s="29"/>
+      <c r="G219" s="9"/>
+      <c r="I219" s="15"/>
     </row>
     <row r="220" spans="3:9">
       <c r="D220" s="1" t="s">
@@ -3806,43 +3976,43 @@
       <c r="F220" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G220" s="15"/>
-      <c r="I220" s="16"/>
+      <c r="G220" s="14"/>
+      <c r="I220" s="15"/>
     </row>
     <row r="221" spans="3:9">
       <c r="C221" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D221" s="10"/>
-      <c r="E221" s="10">
+      <c r="D221" s="9"/>
+      <c r="E221" s="9">
         <f>AVERAGE(E214:E216)</f>
         <v>0.52091767390568999</v>
       </c>
-      <c r="F221" s="10">
+      <c r="F221" s="9">
         <f>AVERAGE(F214:F216)</f>
         <v>0.51417005062103194</v>
       </c>
-      <c r="G221" s="30"/>
-      <c r="I221" s="16"/>
+      <c r="G221" s="29"/>
+      <c r="I221" s="15"/>
     </row>
     <row r="222" spans="3:9">
-      <c r="C222" s="36"/>
+      <c r="C222" s="31"/>
       <c r="D222" s="1"/>
-      <c r="E222" s="15"/>
-      <c r="F222" s="10"/>
-      <c r="G222" s="30"/>
-      <c r="I222" s="16"/>
+      <c r="E222" s="14"/>
+      <c r="F222" s="9"/>
+      <c r="G222" s="29"/>
+      <c r="I222" s="15"/>
     </row>
     <row r="223" spans="3:9">
-      <c r="C223" s="36"/>
+      <c r="C223" s="31"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="15"/>
+      <c r="E223" s="14"/>
       <c r="F223" s="5"/>
       <c r="G223" s="5"/>
-      <c r="I223" s="16"/>
-    </row>
-    <row r="226" spans="3:9" ht="15.75" thickBot="1">
-      <c r="F226" s="13" t="s">
+      <c r="I223" s="15"/>
+    </row>
+    <row r="226" spans="3:9" ht="15" thickBot="1">
+      <c r="F226" s="12" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3863,13 +4033,13 @@
       </c>
     </row>
     <row r="229" spans="3:9">
-      <c r="E229" s="37">
+      <c r="E229" s="32">
         <v>0.546558678150177</v>
       </c>
-      <c r="F229" s="37">
+      <c r="F229" s="32">
         <v>0.56275302171707098</v>
       </c>
-      <c r="G229" s="28"/>
+      <c r="G229" s="27"/>
     </row>
     <row r="230" spans="3:9">
       <c r="E230" s="1"/>
@@ -3877,28 +4047,28 @@
       <c r="G230" s="1"/>
     </row>
     <row r="231" spans="3:9">
-      <c r="C231" s="35"/>
+      <c r="C231" s="30"/>
       <c r="D231" s="1"/>
-      <c r="E231" s="10"/>
-      <c r="F231" s="29"/>
-      <c r="G231" s="12"/>
-      <c r="I231" s="16"/>
+      <c r="E231" s="9"/>
+      <c r="F231" s="28"/>
+      <c r="G231" s="11"/>
+      <c r="I231" s="15"/>
     </row>
     <row r="232" spans="3:9">
-      <c r="C232" s="36"/>
+      <c r="C232" s="31"/>
       <c r="D232" s="1"/>
-      <c r="E232" s="10"/>
-      <c r="F232" s="30"/>
-      <c r="G232" s="10"/>
-      <c r="I232" s="16"/>
+      <c r="E232" s="9"/>
+      <c r="F232" s="29"/>
+      <c r="G232" s="9"/>
+      <c r="I232" s="15"/>
     </row>
     <row r="233" spans="3:9">
-      <c r="C233" s="36"/>
+      <c r="C233" s="31"/>
       <c r="D233" s="1"/>
-      <c r="E233" s="15"/>
-      <c r="F233" s="15"/>
-      <c r="G233" s="15"/>
-      <c r="I233" s="16"/>
+      <c r="E233" s="14"/>
+      <c r="F233" s="14"/>
+      <c r="G233" s="14"/>
+      <c r="I233" s="15"/>
     </row>
     <row r="234" spans="3:9">
       <c r="D234" s="1" t="s">
@@ -3910,35 +4080,617 @@
       <c r="F234" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G234" s="30"/>
-      <c r="I234" s="16"/>
+      <c r="G234" s="29"/>
+      <c r="I234" s="15"/>
     </row>
     <row r="235" spans="3:9">
       <c r="C235" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D235" s="10"/>
-      <c r="E235" s="10">
+      <c r="D235" s="9"/>
+      <c r="E235" s="9">
         <f>AVERAGE(E227:E229)</f>
         <v>0.52631578842798843</v>
       </c>
-      <c r="F235" s="10">
+      <c r="F235" s="9">
         <f>AVERAGE(F227:F229)</f>
         <v>0.54790822664896599</v>
       </c>
-      <c r="G235" s="30"/>
-      <c r="I235" s="16"/>
+      <c r="G235" s="29"/>
+      <c r="I235" s="15"/>
     </row>
     <row r="236" spans="3:9">
-      <c r="C236" s="36"/>
+      <c r="C236" s="31"/>
       <c r="D236" s="1"/>
-      <c r="E236" s="15"/>
+      <c r="E236" s="14"/>
       <c r="F236" s="5"/>
       <c r="G236" s="5"/>
-      <c r="I236" s="16"/>
+      <c r="I236" s="15"/>
+    </row>
+    <row r="243" spans="3:13" ht="15" thickBot="1">
+      <c r="C243" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D243" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="E243" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="G243" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="H243" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="I243" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="K243" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="L243" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="M243" s="38" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="244" spans="3:13">
+      <c r="C244" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D244" s="40">
+        <v>0.7</v>
+      </c>
+      <c r="E244" s="41">
+        <v>0.76</v>
+      </c>
+      <c r="G244" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H244" s="40">
+        <v>0.69</v>
+      </c>
+      <c r="I244" s="41">
+        <v>0.76</v>
+      </c>
+      <c r="K244" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="L244" s="40">
+        <v>0.71</v>
+      </c>
+      <c r="M244" s="41">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="245" spans="3:13">
+      <c r="C245" s="39"/>
+      <c r="D245" s="40">
+        <v>0.69</v>
+      </c>
+      <c r="E245" s="41">
+        <v>0.87</v>
+      </c>
+      <c r="G245" s="39"/>
+      <c r="H245" s="40">
+        <v>0.69</v>
+      </c>
+      <c r="I245" s="41">
+        <v>0.77</v>
+      </c>
+      <c r="K245" s="39"/>
+      <c r="L245" s="40">
+        <v>0.68</v>
+      </c>
+      <c r="M245" s="41">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="246" spans="3:13">
+      <c r="C246" s="39"/>
+      <c r="D246" s="40">
+        <v>0.7</v>
+      </c>
+      <c r="E246" s="41">
+        <v>0.84</v>
+      </c>
+      <c r="G246" s="39"/>
+      <c r="H246" s="40">
+        <v>0.72</v>
+      </c>
+      <c r="I246" s="41">
+        <v>0.81</v>
+      </c>
+      <c r="K246" s="39"/>
+      <c r="L246" s="40">
+        <v>0.7</v>
+      </c>
+      <c r="M246" s="41">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="247" spans="3:13">
+      <c r="C247" s="39"/>
+      <c r="D247" s="47">
+        <v>0.65</v>
+      </c>
+      <c r="E247" s="49">
+        <v>0.88</v>
+      </c>
+      <c r="G247" s="39"/>
+      <c r="H247" s="42">
+        <f>AVERAGE(H244:H246)</f>
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="I247" s="43">
+        <f>AVERAGE(I244:I246)</f>
+        <v>0.77999999999999992</v>
+      </c>
+      <c r="K247" s="39"/>
+      <c r="L247" s="42">
+        <f>AVERAGE(L244:L246)</f>
+        <v>0.69666666666666666</v>
+      </c>
+      <c r="M247" s="43">
+        <f>AVERAGE(M244:M246)</f>
+        <v>0.79333333333333333</v>
+      </c>
+    </row>
+    <row r="248" spans="3:13">
+      <c r="C248" s="39"/>
+      <c r="D248" s="48">
+        <v>0.7</v>
+      </c>
+      <c r="E248" s="50">
+        <v>0.77</v>
+      </c>
+      <c r="G248" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H248" s="40">
+        <v>0.78</v>
+      </c>
+      <c r="I248" s="41">
+        <v>0.82</v>
+      </c>
+      <c r="K248" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="L248" s="40">
+        <v>0.72</v>
+      </c>
+      <c r="M248" s="41">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="249" spans="3:13">
+      <c r="C249" s="39"/>
+      <c r="D249" s="42">
+        <f>AVERAGE(D244:D248)</f>
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="E249" s="43">
+        <f>AVERAGE(E244:E248)</f>
+        <v>0.82399999999999984</v>
+      </c>
+      <c r="G249" s="39"/>
+      <c r="H249" s="40">
+        <v>0.73</v>
+      </c>
+      <c r="I249" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="K249" s="39"/>
+      <c r="L249" s="40">
+        <v>0.72</v>
+      </c>
+      <c r="M249" s="41">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="250" spans="3:13">
+      <c r="C250" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250" s="48">
+        <v>0.72</v>
+      </c>
+      <c r="E250" s="50">
+        <v>0.81</v>
+      </c>
+      <c r="G250" s="39"/>
+      <c r="H250" s="40">
+        <v>0.75</v>
+      </c>
+      <c r="I250" s="41">
+        <v>0.84</v>
+      </c>
+      <c r="K250" s="39"/>
+      <c r="L250" s="40">
+        <v>0.73</v>
+      </c>
+      <c r="M250" s="41">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="251" spans="3:13">
+      <c r="C251" s="39"/>
+      <c r="D251" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="E251" s="49">
+        <v>0.84</v>
+      </c>
+      <c r="G251" s="44"/>
+      <c r="H251" s="45">
+        <f>AVERAGE(H248:H250)</f>
+        <v>0.7533333333333333</v>
+      </c>
+      <c r="I251" s="46">
+        <f>AVERAGE(I248:I250)</f>
+        <v>0.82</v>
+      </c>
+      <c r="K251" s="39"/>
+      <c r="L251" s="40">
+        <v>0.79</v>
+      </c>
+      <c r="M251" s="41">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="252" spans="3:13">
+      <c r="C252" s="39"/>
+      <c r="D252" s="40">
+        <v>0.71</v>
+      </c>
+      <c r="E252" s="41">
+        <v>0.74</v>
+      </c>
+      <c r="K252" s="44"/>
+      <c r="L252" s="45">
+        <f>AVERAGE(L248:L251)</f>
+        <v>0.74</v>
+      </c>
+      <c r="M252" s="46">
+        <f>AVERAGE(M248:M251)</f>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="253" spans="3:13">
+      <c r="C253" s="39"/>
+      <c r="D253" s="40">
+        <v>0.74</v>
+      </c>
+      <c r="E253" s="41">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="254" spans="3:13">
+      <c r="C254" s="39"/>
+      <c r="D254" s="40">
+        <v>0.75</v>
+      </c>
+      <c r="E254" s="41">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="255" spans="3:13">
+      <c r="C255" s="44"/>
+      <c r="D255" s="45">
+        <f>AVERAGE(D250:D254)</f>
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="E255" s="46">
+        <f>AVERAGE(E250:E254)</f>
+        <v>0.78799999999999992</v>
+      </c>
+    </row>
+    <row r="256" spans="3:13">
+      <c r="G256" t="s">
+        <v>216</v>
+      </c>
+      <c r="H256">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="3:11">
+      <c r="G257" t="s">
+        <v>217</v>
+      </c>
+      <c r="H257">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="3:11">
+      <c r="G258" t="s">
+        <v>218</v>
+      </c>
+      <c r="H258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="3:11">
+      <c r="C259" t="s">
+        <v>215</v>
+      </c>
+      <c r="G259" t="s">
+        <v>219</v>
+      </c>
+      <c r="H259">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="3:11">
+      <c r="G260" t="s">
+        <v>220</v>
+      </c>
+      <c r="H260">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="3:11">
+      <c r="C261" t="s">
+        <v>222</v>
+      </c>
+      <c r="G261" t="s">
+        <v>221</v>
+      </c>
+      <c r="H261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="3:11">
+      <c r="C262" t="s">
+        <v>1</v>
+      </c>
+      <c r="D262" s="9">
+        <f>AVERAGE(D23,F61,F63,F65,E78,F82,F84,F86,E99,F103,F105,F107,E120,F124,F126,F128,E161,F145,F147,E171)</f>
+        <v>0.68779352169207342</v>
+      </c>
+      <c r="H262">
+        <f>SUM(H256:H261)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="263" spans="3:11">
+      <c r="C263" t="s">
+        <v>2</v>
+      </c>
+      <c r="D263" s="9">
+        <f>AVERAGE(E23,G61,G63,G65,F78,G82,G84,G86,F99,G103,G105,G107,F120,G124,G126,G128,F161,G145,G147,F171)</f>
+        <v>0.69571524896039283</v>
+      </c>
+    </row>
+    <row r="264" spans="3:11">
+      <c r="G264">
+        <v>1</v>
+      </c>
+      <c r="H264" s="1">
+        <f>H262-G264</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="265" spans="3:11">
+      <c r="G265" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="266" spans="3:11">
+      <c r="C266" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="267" spans="3:11">
+      <c r="C267" t="s">
+        <v>29</v>
+      </c>
+      <c r="D267" s="9">
+        <f>AVERAGE(D23:E23,E78:F78,E99:F99,E120:F120)</f>
+        <v>0.72803643494844383</v>
+      </c>
+      <c r="E267" t="s">
+        <v>237</v>
+      </c>
+      <c r="G267" t="s">
+        <v>216</v>
+      </c>
+      <c r="H267">
+        <v>2</v>
+      </c>
+      <c r="J267" t="s">
+        <v>216</v>
+      </c>
+      <c r="K267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="3:11">
+      <c r="C268" t="s">
+        <v>224</v>
+      </c>
+      <c r="D268" s="9">
+        <f>AVERAGE(F61:G61,F103:G103,F145:G145,F82:G82,F124:G124,)</f>
+        <v>0.59790209790209747</v>
+      </c>
+      <c r="G268" t="s">
+        <v>217</v>
+      </c>
+      <c r="H268">
+        <v>2</v>
+      </c>
+      <c r="J268" t="s">
+        <v>217</v>
+      </c>
+      <c r="K268">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="3:11">
+      <c r="C269" t="s">
+        <v>225</v>
+      </c>
+      <c r="D269" s="9">
+        <f>AVERAGE(F63:G63,F84:G84,F105:G105,F126:G126,F147:G147,)</f>
+        <v>0.65509753404490212</v>
+      </c>
+      <c r="G269" t="s">
+        <v>218</v>
+      </c>
+      <c r="H269">
+        <v>2</v>
+      </c>
+      <c r="J269" t="s">
+        <v>218</v>
+      </c>
+      <c r="K269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="3:11">
+      <c r="C270" t="s">
+        <v>27</v>
+      </c>
+      <c r="D270" s="9">
+        <f>AVERAGE(F65:G65,F86:G86,F107:G107,F128:G128)</f>
+        <v>0.67925101214574868</v>
+      </c>
+      <c r="E270" t="s">
+        <v>227</v>
+      </c>
+      <c r="G270" t="s">
+        <v>219</v>
+      </c>
+      <c r="H270">
+        <v>2</v>
+      </c>
+      <c r="J270" t="s">
+        <v>219</v>
+      </c>
+      <c r="K270">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="3:11">
+      <c r="G271" t="s">
+        <v>220</v>
+      </c>
+      <c r="H271">
+        <v>2</v>
+      </c>
+      <c r="J271" t="s">
+        <v>226</v>
+      </c>
+      <c r="K271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="3:11">
+      <c r="G272" t="s">
+        <v>221</v>
+      </c>
+      <c r="H272">
+        <v>2</v>
+      </c>
+      <c r="K272" s="1">
+        <f ca="1">SUM(K267:K272)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="3:10">
+      <c r="H273" s="1">
+        <f>SUM(H267:H272)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="275" spans="3:10">
+      <c r="G275" t="s">
+        <v>29</v>
+      </c>
+      <c r="J275" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="279" spans="3:10">
+      <c r="C279" t="s">
+        <v>229</v>
+      </c>
+      <c r="D279" s="9">
+        <f>AVERAGE(D23:E23,F61:G61,F63:G63,F65:G65,)</f>
+        <v>0.63063427867837885</v>
+      </c>
+      <c r="E279">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="3:10">
+      <c r="C280" t="s">
+        <v>230</v>
+      </c>
+      <c r="D280" s="9">
+        <f>AVERAGE(E78:F78,F82:G82,F84:G84,F86:G86,)</f>
+        <v>0.5609086815966603</v>
+      </c>
+      <c r="E280">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="3:10">
+      <c r="C281" t="s">
+        <v>231</v>
+      </c>
+      <c r="D281" s="9">
+        <f>AVERAGE(E99:F99,F103:G103,F105:G105,F107:G107)</f>
+        <v>0.72631578631246574</v>
+      </c>
+      <c r="E281">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="3:10">
+      <c r="C282" t="s">
+        <v>232</v>
+      </c>
+      <c r="D282" s="9">
+        <f>AVERAGE(E120:F120,F124:G124,F126:G126,F128:G128)</f>
+        <v>0.70951417055327859</v>
+      </c>
+      <c r="E282">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="3:10">
+      <c r="C283" t="s">
+        <v>233</v>
+      </c>
+      <c r="D283" s="9">
+        <f>AVERAGE(F145:G145,F147:G147,E161:F161,E171:F171,)</f>
+        <v>0.6066276795164468</v>
+      </c>
+      <c r="E283" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="284" spans="3:10">
+      <c r="C284" t="s">
+        <v>234</v>
+      </c>
+      <c r="D284" s="9">
+        <f>AVERAGE(E201:F201,F205:G205,F207:G207,E221:F221,E235:F235,)</f>
+        <v>0.50198748587479713</v>
+      </c>
+      <c r="E284" t="s">
+        <v>236</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E203:G203"/>
+    <mergeCell ref="C205:C210"/>
+    <mergeCell ref="E164:G164"/>
+    <mergeCell ref="C166:C171"/>
+    <mergeCell ref="E188:G188"/>
     <mergeCell ref="E143:G143"/>
     <mergeCell ref="C145:C150"/>
     <mergeCell ref="C2:E2"/>
@@ -3951,11 +4703,6 @@
     <mergeCell ref="C82:C87"/>
     <mergeCell ref="E101:G101"/>
     <mergeCell ref="C103:C108"/>
-    <mergeCell ref="E203:G203"/>
-    <mergeCell ref="C205:C210"/>
-    <mergeCell ref="E164:G164"/>
-    <mergeCell ref="C166:C171"/>
-    <mergeCell ref="E188:G188"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3970,7 +4717,7 @@
       <selection activeCell="B2" sqref="B2:AB35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add calculations in algorithms results
</commit_message>
<xml_diff>
--- a/algorithms_results.xlsx
+++ b/algorithms_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Studia\mgr\praca_magisterska\auth-smile-classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162E5F50-67E8-42F9-B4E7-2198815432B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBFB0B0-C162-4ADF-99F9-B910B52CD071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="239">
   <si>
     <t>scaled</t>
   </si>
@@ -750,19 +750,23 @@
     <t>bez BOSSVS</t>
   </si>
   <si>
-    <t>tylko domysln.</t>
+    <t>36-40</t>
+  </si>
+  <si>
+    <t>tylko domysln., ale bez twarzy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,16 +881,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="JetBrains Mono"/>
@@ -900,8 +894,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -911,6 +921,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1014,11 +1034,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1034,20 +1056,18 @@
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1068,6 +1088,17 @@
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1080,25 +1111,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="17" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutralny" xfId="3" builtinId="28"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Zły" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1378,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AL284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="H284" sqref="H284"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="I278" sqref="I278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1394,11 +1415,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
@@ -1412,7 +1433,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="44" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -1432,7 +1453,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="35"/>
+      <c r="A5" s="44"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -1450,7 +1471,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="35"/>
+      <c r="A6" s="44"/>
       <c r="B6">
         <v>2</v>
       </c>
@@ -1468,7 +1489,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="35"/>
+      <c r="A7" s="44"/>
       <c r="B7">
         <v>3</v>
       </c>
@@ -1486,7 +1507,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="35"/>
+      <c r="A8" s="44"/>
       <c r="B8">
         <v>4</v>
       </c>
@@ -1504,7 +1525,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="35"/>
+      <c r="A9" s="44"/>
       <c r="B9">
         <v>5</v>
       </c>
@@ -1596,11 +1617,11 @@
         <f>AVERAGE(C25:C29)</f>
         <v>0.69311741590499831</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="46">
         <f>AVERAGE(D25:D29)</f>
         <v>0.74574898481368956</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="47">
         <f>AVERAGE(E25:E29)</f>
         <v>0.76275304555892887</v>
       </c>
@@ -1776,12 +1797,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="7:25">
+    <row r="35" spans="3:25">
       <c r="G35" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:25">
+    <row r="37" spans="3:25">
       <c r="G37" t="s">
         <v>30</v>
       </c>
@@ -1798,7 +1819,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="7:25">
+    <row r="39" spans="3:25">
+      <c r="C39" s="9"/>
       <c r="G39" t="s">
         <v>53</v>
       </c>
@@ -1815,7 +1837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="7:25">
+    <row r="40" spans="3:25">
       <c r="G40" t="s">
         <v>54</v>
       </c>
@@ -1832,7 +1854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="7:25">
+    <row r="42" spans="3:25">
       <c r="G42" t="s">
         <v>55</v>
       </c>
@@ -1849,7 +1871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="7:25">
+    <row r="43" spans="3:25">
       <c r="G43" t="s">
         <v>56</v>
       </c>
@@ -1866,7 +1888,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="7:25">
+    <row r="44" spans="3:25">
       <c r="G44" t="s">
         <v>57</v>
       </c>
@@ -1883,12 +1905,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="7:25">
+    <row r="46" spans="3:25">
       <c r="G46" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="7:25">
+    <row r="48" spans="3:25">
       <c r="G48" t="s">
         <v>30</v>
       </c>
@@ -1996,11 +2018,11 @@
       </c>
     </row>
     <row r="59" spans="3:25">
-      <c r="E59" s="33" t="s">
+      <c r="E59" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
     </row>
     <row r="60" spans="3:25">
       <c r="E60" s="1" t="s">
@@ -2014,7 +2036,7 @@
       </c>
     </row>
     <row r="61" spans="3:25">
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="1">
@@ -2029,7 +2051,7 @@
       <c r="G61" s="11">
         <v>0.68016194331983804</v>
       </c>
-      <c r="I61" s="15" t="s">
+      <c r="I61" s="14" t="s">
         <v>23</v>
       </c>
       <c r="M61" t="s">
@@ -2037,7 +2059,7 @@
       </c>
     </row>
     <row r="62" spans="3:25">
-      <c r="C62" s="34"/>
+      <c r="C62" s="43"/>
       <c r="D62" s="1">
         <v>1</v>
       </c>
@@ -2050,7 +2072,7 @@
       <c r="G62" s="9">
         <v>0.59676113360323801</v>
       </c>
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M62" t="s">
@@ -2058,7 +2080,7 @@
       </c>
     </row>
     <row r="63" spans="3:25">
-      <c r="C63" s="34"/>
+      <c r="C63" s="43"/>
       <c r="D63" s="1">
         <v>2</v>
       </c>
@@ -2068,15 +2090,15 @@
       <c r="F63" s="10">
         <v>0.72793522267206401</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="46">
         <v>0.75748987854251004</v>
       </c>
-      <c r="I63" s="15" t="s">
+      <c r="I63" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="3:25">
-      <c r="C64" s="34"/>
+      <c r="C64" s="43"/>
       <c r="D64" s="1">
         <v>3</v>
       </c>
@@ -2089,7 +2111,7 @@
       <c r="G64" s="8">
         <v>0.70526315789473604</v>
       </c>
-      <c r="I64" s="15" t="s">
+      <c r="I64" s="14" t="s">
         <v>26</v>
       </c>
       <c r="M64" t="s">
@@ -2097,7 +2119,7 @@
       </c>
     </row>
     <row r="65" spans="3:9">
-      <c r="C65" s="34"/>
+      <c r="C65" s="43"/>
       <c r="D65" s="1">
         <v>4</v>
       </c>
@@ -2110,12 +2132,12 @@
       <c r="G65" s="8">
         <v>0.68421052631578905</v>
       </c>
-      <c r="I65" s="15" t="s">
+      <c r="I65" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="66" spans="3:9">
-      <c r="C66" s="34"/>
+      <c r="C66" s="43"/>
       <c r="D66" s="1">
         <v>5</v>
       </c>
@@ -2128,7 +2150,7 @@
       <c r="G66" s="9">
         <v>0.65789473684210498</v>
       </c>
-      <c r="I66" s="15" t="s">
+      <c r="I66" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2224,11 +2246,11 @@
       </c>
     </row>
     <row r="80" spans="3:9">
-      <c r="E80" s="33" t="s">
+      <c r="E80" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="42"/>
     </row>
     <row r="81" spans="3:33">
       <c r="E81" s="1" t="s">
@@ -2242,7 +2264,7 @@
       </c>
     </row>
     <row r="82" spans="3:33">
-      <c r="C82" s="34" t="s">
+      <c r="C82" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="1">
@@ -2251,54 +2273,54 @@
       <c r="E82" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F82" s="24">
+      <c r="F82" s="22">
         <v>0.56356275303643699</v>
       </c>
-      <c r="G82" s="23">
+      <c r="G82" s="21">
         <v>0.58744939271255003</v>
       </c>
-      <c r="I82" s="15" t="s">
+      <c r="I82" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="83" spans="3:33">
-      <c r="C83" s="35"/>
+      <c r="C83" s="44"/>
       <c r="D83" s="1">
         <v>1</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F83" s="24">
+      <c r="F83" s="22">
         <v>0.50404858299595101</v>
       </c>
       <c r="G83" s="5">
         <v>0.52307692307692299</v>
       </c>
-      <c r="I83" s="15" t="s">
+      <c r="I83" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="84" spans="3:33">
-      <c r="C84" s="35"/>
+      <c r="C84" s="44"/>
       <c r="D84" s="1">
         <v>2</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E84" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F84" s="24">
+      <c r="F84" s="22">
         <v>0.66437246963562702</v>
       </c>
-      <c r="G84" s="24">
+      <c r="G84" s="22">
         <v>0.65546558704453395</v>
       </c>
-      <c r="I84" s="15" t="s">
+      <c r="I84" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="3:33">
-      <c r="C85" s="35"/>
+      <c r="C85" s="44"/>
       <c r="D85" s="1">
         <v>3</v>
       </c>
@@ -2308,37 +2330,37 @@
       <c r="F85" s="5">
         <v>0.58461538461538398</v>
       </c>
-      <c r="G85" s="24">
+      <c r="G85" s="22">
         <v>0.60485829959514104</v>
       </c>
-      <c r="I85" s="15" t="s">
+      <c r="I85" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="86" spans="3:33">
-      <c r="C86" s="35"/>
+      <c r="C86" s="44"/>
       <c r="D86" s="1">
         <v>4</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="13" t="s">
         <v>103</v>
       </c>
       <c r="F86" s="5">
         <v>0.63441295546558696</v>
       </c>
-      <c r="G86" s="24">
+      <c r="G86" s="22">
         <v>0.61417004048582902</v>
       </c>
-      <c r="I86" s="15" t="s">
+      <c r="I86" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="87" spans="3:33">
-      <c r="C87" s="35"/>
+      <c r="C87" s="44"/>
       <c r="D87" s="1">
         <v>5</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="13" t="s">
         <v>104</v>
       </c>
       <c r="F87" s="5">
@@ -2347,7 +2369,7 @@
       <c r="G87" s="5">
         <v>0.540485829959514</v>
       </c>
-      <c r="I87" s="15" t="s">
+      <c r="I87" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2366,6 +2388,9 @@
       <c r="F92" s="5">
         <v>0.73279350996017401</v>
       </c>
+      <c r="G92" t="s">
+        <v>237</v>
+      </c>
       <c r="H92" s="1" t="s">
         <v>1</v>
       </c>
@@ -2502,7 +2527,7 @@
         <f>AVERAGE(E92:E96)</f>
         <v>0.73279350996017367</v>
       </c>
-      <c r="F99" s="9">
+      <c r="F99" s="46">
         <f>AVERAGE(F92:F96)</f>
         <v>0.76518217325210514</v>
       </c>
@@ -2546,11 +2571,11 @@
       </c>
     </row>
     <row r="101" spans="3:33">
-      <c r="E101" s="33" t="s">
+      <c r="E101" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F101" s="33"/>
-      <c r="G101" s="33"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
       <c r="H101" t="s">
         <v>113</v>
       </c>
@@ -2582,100 +2607,100 @@
       </c>
     </row>
     <row r="103" spans="3:33">
-      <c r="C103" s="34" t="s">
+      <c r="C103" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
       </c>
       <c r="E103" s="9"/>
-      <c r="F103" s="22">
+      <c r="F103" s="26">
         <v>0.68623481781376505</v>
       </c>
-      <c r="G103" s="23">
+      <c r="G103" s="11">
         <v>0.67004048582995901</v>
       </c>
-      <c r="I103" s="15" t="s">
+      <c r="I103" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="104" spans="3:33">
-      <c r="C104" s="35"/>
+      <c r="C104" s="44"/>
       <c r="D104" s="1">
         <v>1</v>
       </c>
       <c r="E104" s="9"/>
-      <c r="F104" s="24">
+      <c r="F104" s="13">
         <v>0.54008097165991897</v>
       </c>
-      <c r="G104" s="5">
+      <c r="G104" s="9">
         <v>0.61740890688259098</v>
       </c>
-      <c r="I104" s="15" t="s">
+      <c r="I104" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="105" spans="3:33">
-      <c r="C105" s="35"/>
+      <c r="C105" s="44"/>
       <c r="D105" s="1">
         <v>2</v>
       </c>
-      <c r="E105" s="14"/>
-      <c r="F105" s="24">
+      <c r="E105" s="13"/>
+      <c r="F105" s="46">
         <v>0.76194331983805597</v>
       </c>
-      <c r="G105" s="24">
+      <c r="G105" s="47">
         <v>0.76315789473684204</v>
       </c>
-      <c r="I105" s="15" t="s">
+      <c r="I105" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="106" spans="3:33">
-      <c r="C106" s="35"/>
+      <c r="C106" s="44"/>
       <c r="D106" s="1">
         <v>3</v>
       </c>
       <c r="E106" s="9"/>
-      <c r="F106" s="5">
+      <c r="F106" s="9">
         <v>0.68906882591093099</v>
       </c>
-      <c r="G106" s="24">
+      <c r="G106" s="13">
         <v>0.70202429149797496</v>
       </c>
-      <c r="I106" s="15" t="s">
+      <c r="I106" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="107" spans="3:33">
-      <c r="C107" s="35"/>
+      <c r="C107" s="44"/>
       <c r="D107" s="1">
         <v>4</v>
       </c>
-      <c r="E107" s="14"/>
-      <c r="F107" s="5">
+      <c r="E107" s="13"/>
+      <c r="F107" s="9">
         <v>0.708502024291498</v>
       </c>
-      <c r="G107" s="24">
+      <c r="G107" s="13">
         <v>0.72267206477732704</v>
       </c>
-      <c r="I107" s="15" t="s">
+      <c r="I107" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="108" spans="3:33">
-      <c r="C108" s="35"/>
+      <c r="C108" s="44"/>
       <c r="D108" s="1">
         <v>5</v>
       </c>
-      <c r="E108" s="14"/>
-      <c r="F108" s="5">
+      <c r="E108" s="13"/>
+      <c r="F108" s="9">
         <v>0.63643724696356196</v>
       </c>
-      <c r="G108" s="5">
+      <c r="G108" s="9">
         <v>0.72550607287449398</v>
       </c>
-      <c r="I108" s="15" t="s">
+      <c r="I108" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2839,7 +2864,7 @@
         <f>AVERAGE(E113:E117)</f>
         <v>0.72874493598937939</v>
       </c>
-      <c r="F120" s="9">
+      <c r="F120" s="46">
         <f>AVERAGE(F113:F117)</f>
         <v>0.760323894023895</v>
       </c>
@@ -2889,11 +2914,11 @@
       </c>
     </row>
     <row r="122" spans="3:38">
-      <c r="E122" s="33" t="s">
+      <c r="E122" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F122" s="33"/>
-      <c r="G122" s="33"/>
+      <c r="F122" s="42"/>
+      <c r="G122" s="42"/>
       <c r="H122" t="s">
         <v>133</v>
       </c>
@@ -2928,57 +2953,57 @@
       </c>
     </row>
     <row r="124" spans="3:38">
-      <c r="C124" s="34" t="s">
+      <c r="C124" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="1">
         <v>0</v>
       </c>
       <c r="E124" s="9"/>
-      <c r="F124" s="16">
+      <c r="F124" s="15">
         <v>0.65101214574898703</v>
       </c>
       <c r="G124" s="11">
         <v>0.66315789473684195</v>
       </c>
-      <c r="I124" s="15" t="s">
+      <c r="I124" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="125" spans="3:38">
-      <c r="C125" s="35"/>
+      <c r="C125" s="44"/>
       <c r="D125" s="1">
         <v>1</v>
       </c>
       <c r="E125" s="9"/>
-      <c r="F125" s="14">
+      <c r="F125" s="13">
         <v>0.50931174089068798</v>
       </c>
       <c r="G125" s="9">
         <v>0.54089068825910902</v>
       </c>
-      <c r="I125" s="15" t="s">
+      <c r="I125" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="3:38">
-      <c r="C126" s="35"/>
+      <c r="C126" s="44"/>
       <c r="D126" s="1">
         <v>2</v>
       </c>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14">
+      <c r="E126" s="13"/>
+      <c r="F126" s="13">
         <v>0.72550607287449398</v>
       </c>
-      <c r="G126" s="14">
+      <c r="G126" s="13">
         <v>0.72186234817813699</v>
       </c>
-      <c r="I126" s="15" t="s">
+      <c r="I126" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="127" spans="3:38">
-      <c r="C127" s="35"/>
+      <c r="C127" s="44"/>
       <c r="D127" s="1">
         <v>3</v>
       </c>
@@ -2986,42 +3011,42 @@
       <c r="F127" s="9">
         <v>0.675708502024291</v>
       </c>
-      <c r="G127" s="14">
+      <c r="G127" s="13">
         <v>0.67489878542510096</v>
       </c>
-      <c r="I127" s="15" t="s">
+      <c r="I127" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="128" spans="3:38">
-      <c r="C128" s="35"/>
+      <c r="C128" s="44"/>
       <c r="D128" s="1">
         <v>4</v>
       </c>
-      <c r="E128" s="14"/>
+      <c r="E128" s="13"/>
       <c r="F128" s="9">
         <v>0.7</v>
       </c>
-      <c r="G128" s="14">
+      <c r="G128" s="13">
         <v>0.72550607287449398</v>
       </c>
-      <c r="I128" s="15" t="s">
+      <c r="I128" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="129" spans="3:22">
-      <c r="C129" s="35"/>
+      <c r="C129" s="44"/>
       <c r="D129" s="1">
         <v>5</v>
       </c>
-      <c r="E129" s="14"/>
+      <c r="E129" s="13"/>
       <c r="F129" s="9">
         <v>0.62591093117408902</v>
       </c>
       <c r="G129" s="9">
         <v>0.69068825910931098</v>
       </c>
-      <c r="I129" s="15" t="s">
+      <c r="I129" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3157,11 +3182,11 @@
       </c>
     </row>
     <row r="143" spans="3:22">
-      <c r="E143" s="33" t="s">
+      <c r="E143" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F143" s="33"/>
-      <c r="G143" s="33"/>
+      <c r="F143" s="42"/>
+      <c r="G143" s="42"/>
       <c r="L143" t="s">
         <v>154</v>
       </c>
@@ -3184,57 +3209,57 @@
       </c>
     </row>
     <row r="145" spans="3:24">
-      <c r="C145" s="34" t="s">
+      <c r="C145" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D145" s="1">
         <v>0</v>
       </c>
       <c r="E145" s="9"/>
-      <c r="F145" s="28">
+      <c r="F145" s="26">
         <v>0.70526315789473604</v>
       </c>
       <c r="G145" s="11">
         <v>0.69716599190283401</v>
       </c>
-      <c r="I145" s="15" t="s">
+      <c r="I145" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="146" spans="3:24">
-      <c r="C146" s="35"/>
+      <c r="C146" s="44"/>
       <c r="D146" s="1">
         <v>1</v>
       </c>
       <c r="E146" s="9"/>
-      <c r="F146" s="17" t="s">
+      <c r="F146" s="16" t="s">
         <v>186</v>
       </c>
       <c r="G146" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I146" s="15" t="s">
+      <c r="I146" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="147" spans="3:24">
-      <c r="C147" s="35"/>
+      <c r="C147" s="44"/>
       <c r="D147" s="1">
         <v>2</v>
       </c>
-      <c r="E147" s="14"/>
-      <c r="F147" s="14">
+      <c r="E147" s="13"/>
+      <c r="F147" s="13">
         <v>0.72024291497975701</v>
       </c>
-      <c r="G147" s="14">
+      <c r="G147" s="13">
         <v>0.70809716599190198</v>
       </c>
-      <c r="I147" s="15" t="s">
+      <c r="I147" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="148" spans="3:24">
-      <c r="C148" s="35"/>
+      <c r="C148" s="44"/>
       <c r="D148" s="1">
         <v>3</v>
       </c>
@@ -3242,42 +3267,42 @@
       <c r="F148" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G148" s="18" t="s">
+      <c r="G148" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="I148" s="15" t="s">
+      <c r="I148" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="149" spans="3:24">
-      <c r="C149" s="35"/>
+      <c r="C149" s="44"/>
       <c r="D149" s="1">
         <v>4</v>
       </c>
-      <c r="E149" s="14"/>
+      <c r="E149" s="13"/>
       <c r="F149" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G149" s="17" t="s">
+      <c r="G149" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I149" s="15" t="s">
+      <c r="I149" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="150" spans="3:24">
-      <c r="C150" s="35"/>
+      <c r="C150" s="44"/>
       <c r="D150" s="1">
         <v>5</v>
       </c>
-      <c r="E150" s="14"/>
+      <c r="E150" s="13"/>
       <c r="F150" s="5">
         <v>0.65951417004048496</v>
       </c>
       <c r="G150" s="5">
         <v>0.53886639676113302</v>
       </c>
-      <c r="I150" s="15" t="s">
+      <c r="I150" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3285,7 +3310,7 @@
       <c r="F153" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="I153" s="15" t="s">
+      <c r="I153" s="14" t="s">
         <v>1</v>
       </c>
       <c r="S153" s="1" t="s">
@@ -3434,9 +3459,9 @@
       </c>
     </row>
     <row r="164" spans="3:29">
-      <c r="E164" s="33"/>
-      <c r="F164" s="33"/>
-      <c r="G164" s="33"/>
+      <c r="E164" s="42"/>
+      <c r="F164" s="42"/>
+      <c r="G164" s="42"/>
     </row>
     <row r="165" spans="3:29" ht="15" thickBot="1">
       <c r="E165" t="s">
@@ -3447,7 +3472,7 @@
       </c>
     </row>
     <row r="166" spans="3:29">
-      <c r="C166" s="34"/>
+      <c r="C166" s="43"/>
       <c r="D166" s="1"/>
       <c r="E166" s="5">
         <v>0.65587043762206998</v>
@@ -3463,7 +3488,7 @@
       </c>
     </row>
     <row r="167" spans="3:29">
-      <c r="C167" s="35"/>
+      <c r="C167" s="44"/>
       <c r="D167" s="1"/>
       <c r="E167" s="5">
         <v>0.70445346832275302</v>
@@ -3488,7 +3513,7 @@
       </c>
     </row>
     <row r="168" spans="3:29">
-      <c r="C168" s="35"/>
+      <c r="C168" s="44"/>
       <c r="D168" s="1"/>
       <c r="E168" s="5">
         <v>0.67206478118896396</v>
@@ -3513,11 +3538,11 @@
       </c>
     </row>
     <row r="169" spans="3:29">
-      <c r="C169" s="35"/>
+      <c r="C169" s="44"/>
       <c r="D169" s="1"/>
     </row>
     <row r="170" spans="3:29">
-      <c r="C170" s="35"/>
+      <c r="C170" s="44"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1" t="s">
         <v>1</v>
@@ -3542,7 +3567,7 @@
       </c>
     </row>
     <row r="171" spans="3:29">
-      <c r="C171" s="35"/>
+      <c r="C171" s="44"/>
       <c r="D171" s="1"/>
       <c r="E171" s="9">
         <f>AVERAGE(E166:E168)</f>
@@ -3625,19 +3650,19 @@
       </c>
     </row>
     <row r="181" spans="3:9">
-      <c r="C181" s="21" t="s">
+      <c r="C181" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D181" s="20">
+      <c r="D181" s="19">
         <f>AVERAGE(F61:G61,F82:G82,F103:G103,F124:G124,F145:G145)</f>
         <v>0.65769230769230724</v>
       </c>
-      <c r="E181" s="21">
+      <c r="E181" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="182" spans="3:9">
-      <c r="C182" s="15" t="s">
+      <c r="C182" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D182" s="9">
@@ -3649,14 +3674,14 @@
       </c>
     </row>
     <row r="183" spans="3:9">
-      <c r="C183" s="21" t="s">
+      <c r="C183" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D183" s="20">
+      <c r="D183" s="19">
         <f>AVERAGE(F63:G63,F84:G84,F105:G105,F126:G126,F147:G147)</f>
         <v>0.72060728744939229</v>
       </c>
-      <c r="E183" s="21">
+      <c r="E183" s="20">
         <v>1</v>
       </c>
     </row>
@@ -3673,19 +3698,19 @@
       </c>
     </row>
     <row r="185" spans="3:9">
-      <c r="C185" s="19" t="s">
+      <c r="C185" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D185" s="20">
+      <c r="D185" s="19">
         <f>AVERAGE(F65:G65,F86:G86,F107:G107,F128:G128)</f>
         <v>0.67925101214574868</v>
       </c>
-      <c r="E185" s="21">
+      <c r="E185" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="186" spans="3:9">
-      <c r="C186" s="15" t="s">
+      <c r="C186" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D186" s="9">
@@ -3697,9 +3722,9 @@
       </c>
     </row>
     <row r="188" spans="3:9">
-      <c r="E188" s="33"/>
-      <c r="F188" s="33"/>
-      <c r="G188" s="33"/>
+      <c r="E188" s="42"/>
+      <c r="F188" s="42"/>
+      <c r="G188" s="42"/>
     </row>
     <row r="189" spans="3:9">
       <c r="E189" s="1"/>
@@ -3707,25 +3732,25 @@
       <c r="G189" s="1"/>
     </row>
     <row r="190" spans="3:9">
-      <c r="C190" s="25"/>
+      <c r="C190" s="23"/>
       <c r="D190" s="1"/>
       <c r="E190" s="9"/>
-      <c r="F190" s="16"/>
-      <c r="I190" s="15"/>
+      <c r="F190" s="15"/>
+      <c r="I190" s="14"/>
     </row>
     <row r="191" spans="3:9">
-      <c r="C191" s="26"/>
+      <c r="C191" s="24"/>
       <c r="D191" s="1"/>
       <c r="E191" s="9"/>
-      <c r="F191" s="18"/>
-      <c r="I191" s="15"/>
+      <c r="F191" s="17"/>
+      <c r="I191" s="14"/>
     </row>
     <row r="192" spans="3:9">
-      <c r="C192" s="26"/>
+      <c r="C192" s="24"/>
       <c r="D192" s="1"/>
-      <c r="E192" s="14"/>
-      <c r="F192" s="14"/>
-      <c r="I192" s="15"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="13"/>
+      <c r="I192" s="14"/>
     </row>
     <row r="193" spans="3:9" ht="15" thickBot="1">
       <c r="F193" s="12" t="s">
@@ -3802,11 +3827,11 @@
       </c>
     </row>
     <row r="203" spans="3:9">
-      <c r="E203" s="33" t="s">
+      <c r="E203" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F203" s="33"/>
-      <c r="G203" s="33"/>
+      <c r="F203" s="42"/>
+      <c r="G203" s="42"/>
     </row>
     <row r="204" spans="3:9">
       <c r="E204" s="1" t="s">
@@ -3820,98 +3845,98 @@
       </c>
     </row>
     <row r="205" spans="3:9">
-      <c r="C205" s="34" t="s">
+      <c r="C205" s="43" t="s">
         <v>4</v>
       </c>
       <c r="D205" s="1">
         <v>0</v>
       </c>
       <c r="E205" s="9"/>
-      <c r="F205" s="28">
+      <c r="F205" s="26">
         <v>0.54898785425101204</v>
       </c>
       <c r="G205" s="11">
         <v>0.55182186234817798</v>
       </c>
-      <c r="I205" s="15" t="s">
+      <c r="I205" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="206" spans="3:9">
-      <c r="C206" s="35"/>
+      <c r="C206" s="44"/>
       <c r="D206" s="1">
         <v>1</v>
       </c>
       <c r="E206" s="9"/>
-      <c r="F206" s="29" t="s">
+      <c r="F206" s="27" t="s">
         <v>210</v>
       </c>
       <c r="G206" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="I206" s="15" t="s">
+      <c r="I206" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="207" spans="3:9">
-      <c r="C207" s="35"/>
+      <c r="C207" s="44"/>
       <c r="D207" s="1">
         <v>2</v>
       </c>
-      <c r="E207" s="14"/>
-      <c r="F207" s="14">
+      <c r="E207" s="13"/>
+      <c r="F207" s="13">
         <v>0.61417004048582902</v>
       </c>
-      <c r="G207" s="14">
+      <c r="G207" s="13">
         <v>0.61740890688259098</v>
       </c>
-      <c r="I207" s="15" t="s">
+      <c r="I207" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="208" spans="3:9">
-      <c r="C208" s="35"/>
+      <c r="C208" s="44"/>
       <c r="D208" s="1">
         <v>3</v>
       </c>
       <c r="E208" s="9"/>
       <c r="F208" s="9"/>
-      <c r="G208" s="29" t="s">
+      <c r="G208" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="I208" s="15" t="s">
+      <c r="I208" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="209" spans="3:9">
-      <c r="C209" s="35"/>
+      <c r="C209" s="44"/>
       <c r="D209" s="1">
         <v>4</v>
       </c>
-      <c r="E209" s="14"/>
+      <c r="E209" s="13"/>
       <c r="F209" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G209" s="29" t="s">
+      <c r="G209" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="I209" s="15" t="s">
+      <c r="I209" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="210" spans="3:9">
-      <c r="C210" s="35"/>
+      <c r="C210" s="44"/>
       <c r="D210" s="1">
         <v>5</v>
       </c>
-      <c r="E210" s="14"/>
+      <c r="E210" s="13"/>
       <c r="F210" s="5" t="s">
         <v>210</v>
       </c>
       <c r="G210" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I210" s="15" t="s">
+      <c r="I210" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3937,13 +3962,13 @@
       </c>
     </row>
     <row r="216" spans="3:9">
-      <c r="E216" s="32">
+      <c r="E216" s="30">
         <v>0.48582994937896701</v>
       </c>
-      <c r="F216" s="32">
+      <c r="F216" s="30">
         <v>0.48178136348724299</v>
       </c>
-      <c r="G216" s="27"/>
+      <c r="G216" s="25"/>
     </row>
     <row r="217" spans="3:9">
       <c r="E217" s="1"/>
@@ -3951,20 +3976,20 @@
       <c r="G217" s="1"/>
     </row>
     <row r="218" spans="3:9">
-      <c r="C218" s="30"/>
+      <c r="C218" s="28"/>
       <c r="D218" s="1"/>
       <c r="E218" s="9"/>
-      <c r="F218" s="28"/>
+      <c r="F218" s="26"/>
       <c r="G218" s="11"/>
-      <c r="I218" s="15"/>
+      <c r="I218" s="14"/>
     </row>
     <row r="219" spans="3:9">
-      <c r="C219" s="31"/>
+      <c r="C219" s="29"/>
       <c r="D219" s="1"/>
       <c r="E219" s="9"/>
-      <c r="F219" s="29"/>
+      <c r="F219" s="27"/>
       <c r="G219" s="9"/>
-      <c r="I219" s="15"/>
+      <c r="I219" s="14"/>
     </row>
     <row r="220" spans="3:9">
       <c r="D220" s="1" t="s">
@@ -3976,8 +4001,8 @@
       <c r="F220" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G220" s="14"/>
-      <c r="I220" s="15"/>
+      <c r="G220" s="13"/>
+      <c r="I220" s="14"/>
     </row>
     <row r="221" spans="3:9">
       <c r="C221" s="1" t="s">
@@ -3992,24 +4017,24 @@
         <f>AVERAGE(F214:F216)</f>
         <v>0.51417005062103194</v>
       </c>
-      <c r="G221" s="29"/>
-      <c r="I221" s="15"/>
+      <c r="G221" s="27"/>
+      <c r="I221" s="14"/>
     </row>
     <row r="222" spans="3:9">
-      <c r="C222" s="31"/>
+      <c r="C222" s="29"/>
       <c r="D222" s="1"/>
-      <c r="E222" s="14"/>
+      <c r="E222" s="13"/>
       <c r="F222" s="9"/>
-      <c r="G222" s="29"/>
-      <c r="I222" s="15"/>
+      <c r="G222" s="27"/>
+      <c r="I222" s="14"/>
     </row>
     <row r="223" spans="3:9">
-      <c r="C223" s="31"/>
+      <c r="C223" s="29"/>
       <c r="D223" s="1"/>
-      <c r="E223" s="14"/>
+      <c r="E223" s="13"/>
       <c r="F223" s="5"/>
       <c r="G223" s="5"/>
-      <c r="I223" s="15"/>
+      <c r="I223" s="14"/>
     </row>
     <row r="226" spans="3:9" ht="15" thickBot="1">
       <c r="F226" s="12" t="s">
@@ -4033,13 +4058,13 @@
       </c>
     </row>
     <row r="229" spans="3:9">
-      <c r="E229" s="32">
+      <c r="E229" s="30">
         <v>0.546558678150177</v>
       </c>
-      <c r="F229" s="32">
+      <c r="F229" s="30">
         <v>0.56275302171707098</v>
       </c>
-      <c r="G229" s="27"/>
+      <c r="G229" s="25"/>
     </row>
     <row r="230" spans="3:9">
       <c r="E230" s="1"/>
@@ -4047,28 +4072,28 @@
       <c r="G230" s="1"/>
     </row>
     <row r="231" spans="3:9">
-      <c r="C231" s="30"/>
+      <c r="C231" s="28"/>
       <c r="D231" s="1"/>
       <c r="E231" s="9"/>
-      <c r="F231" s="28"/>
+      <c r="F231" s="26"/>
       <c r="G231" s="11"/>
-      <c r="I231" s="15"/>
+      <c r="I231" s="14"/>
     </row>
     <row r="232" spans="3:9">
-      <c r="C232" s="31"/>
+      <c r="C232" s="29"/>
       <c r="D232" s="1"/>
       <c r="E232" s="9"/>
-      <c r="F232" s="29"/>
+      <c r="F232" s="27"/>
       <c r="G232" s="9"/>
-      <c r="I232" s="15"/>
+      <c r="I232" s="14"/>
     </row>
     <row r="233" spans="3:9">
-      <c r="C233" s="31"/>
+      <c r="C233" s="29"/>
       <c r="D233" s="1"/>
-      <c r="E233" s="14"/>
-      <c r="F233" s="14"/>
-      <c r="G233" s="14"/>
-      <c r="I233" s="15"/>
+      <c r="E233" s="13"/>
+      <c r="F233" s="13"/>
+      <c r="G233" s="13"/>
+      <c r="I233" s="14"/>
     </row>
     <row r="234" spans="3:9">
       <c r="D234" s="1" t="s">
@@ -4080,8 +4105,8 @@
       <c r="F234" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G234" s="29"/>
-      <c r="I234" s="15"/>
+      <c r="G234" s="27"/>
+      <c r="I234" s="14"/>
     </row>
     <row r="235" spans="3:9">
       <c r="C235" s="1" t="s">
@@ -4096,293 +4121,293 @@
         <f>AVERAGE(F227:F229)</f>
         <v>0.54790822664896599</v>
       </c>
-      <c r="G235" s="29"/>
-      <c r="I235" s="15"/>
+      <c r="G235" s="27"/>
+      <c r="I235" s="14"/>
     </row>
     <row r="236" spans="3:9">
-      <c r="C236" s="31"/>
+      <c r="C236" s="29"/>
       <c r="D236" s="1"/>
-      <c r="E236" s="14"/>
+      <c r="E236" s="13"/>
       <c r="F236" s="5"/>
       <c r="G236" s="5"/>
-      <c r="I236" s="15"/>
+      <c r="I236" s="14"/>
     </row>
     <row r="243" spans="3:13" ht="15" thickBot="1">
-      <c r="C243" s="51" t="s">
+      <c r="C243" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D243" s="37" t="s">
+      <c r="D243" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="E243" s="38" t="s">
+      <c r="E243" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="G243" s="51" t="s">
+      <c r="G243" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="H243" s="37" t="s">
+      <c r="H243" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="I243" s="38" t="s">
+      <c r="I243" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="K243" s="51" t="s">
+      <c r="K243" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="L243" s="37" t="s">
+      <c r="L243" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="M243" s="38" t="s">
+      <c r="M243" s="32" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="244" spans="3:13">
-      <c r="C244" s="39" t="s">
+      <c r="C244" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D244" s="40">
+      <c r="D244">
         <v>0.7</v>
       </c>
-      <c r="E244" s="41">
+      <c r="E244" s="34">
         <v>0.76</v>
       </c>
-      <c r="G244" s="39" t="s">
+      <c r="G244" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H244" s="40">
+      <c r="H244">
         <v>0.69</v>
       </c>
-      <c r="I244" s="41">
+      <c r="I244" s="34">
         <v>0.76</v>
       </c>
-      <c r="K244" s="39" t="s">
+      <c r="K244" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="L244" s="40">
+      <c r="L244">
         <v>0.71</v>
       </c>
-      <c r="M244" s="41">
+      <c r="M244" s="34">
         <v>0.82</v>
       </c>
     </row>
     <row r="245" spans="3:13">
-      <c r="C245" s="39"/>
-      <c r="D245" s="40">
+      <c r="C245" s="33"/>
+      <c r="D245">
         <v>0.69</v>
       </c>
-      <c r="E245" s="41">
+      <c r="E245" s="34">
         <v>0.87</v>
       </c>
-      <c r="G245" s="39"/>
-      <c r="H245" s="40">
+      <c r="G245" s="33"/>
+      <c r="H245">
         <v>0.69</v>
       </c>
-      <c r="I245" s="41">
+      <c r="I245" s="34">
         <v>0.77</v>
       </c>
-      <c r="K245" s="39"/>
-      <c r="L245" s="40">
+      <c r="K245" s="33"/>
+      <c r="L245">
         <v>0.68</v>
       </c>
-      <c r="M245" s="41">
+      <c r="M245" s="34">
         <v>0.78</v>
       </c>
     </row>
     <row r="246" spans="3:13">
-      <c r="C246" s="39"/>
-      <c r="D246" s="40">
+      <c r="C246" s="33"/>
+      <c r="D246">
         <v>0.7</v>
       </c>
-      <c r="E246" s="41">
+      <c r="E246" s="34">
         <v>0.84</v>
       </c>
-      <c r="G246" s="39"/>
-      <c r="H246" s="40">
+      <c r="G246" s="33"/>
+      <c r="H246">
         <v>0.72</v>
       </c>
-      <c r="I246" s="41">
+      <c r="I246" s="34">
         <v>0.81</v>
       </c>
-      <c r="K246" s="39"/>
-      <c r="L246" s="40">
+      <c r="K246" s="33"/>
+      <c r="L246">
         <v>0.7</v>
       </c>
-      <c r="M246" s="41">
+      <c r="M246" s="34">
         <v>0.78</v>
       </c>
     </row>
     <row r="247" spans="3:13">
-      <c r="C247" s="39"/>
-      <c r="D247" s="47">
+      <c r="C247" s="33"/>
+      <c r="D247" s="39">
         <v>0.65</v>
       </c>
-      <c r="E247" s="49">
+      <c r="E247" s="40">
         <v>0.88</v>
       </c>
-      <c r="G247" s="39"/>
-      <c r="H247" s="42">
+      <c r="G247" s="33"/>
+      <c r="H247" s="1">
         <f>AVERAGE(H244:H246)</f>
         <v>0.69999999999999984</v>
       </c>
-      <c r="I247" s="43">
+      <c r="I247" s="35">
         <f>AVERAGE(I244:I246)</f>
         <v>0.77999999999999992</v>
       </c>
-      <c r="K247" s="39"/>
-      <c r="L247" s="42">
+      <c r="K247" s="33"/>
+      <c r="L247" s="1">
         <f>AVERAGE(L244:L246)</f>
         <v>0.69666666666666666</v>
       </c>
-      <c r="M247" s="43">
+      <c r="M247" s="35">
         <f>AVERAGE(M244:M246)</f>
         <v>0.79333333333333333</v>
       </c>
     </row>
     <row r="248" spans="3:13">
-      <c r="C248" s="39"/>
-      <c r="D248" s="48">
+      <c r="C248" s="33"/>
+      <c r="D248">
         <v>0.7</v>
       </c>
-      <c r="E248" s="50">
+      <c r="E248" s="34">
         <v>0.77</v>
       </c>
-      <c r="G248" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="H248" s="40">
+      <c r="G248" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H248">
         <v>0.78</v>
       </c>
-      <c r="I248" s="41">
+      <c r="I248" s="34">
         <v>0.82</v>
       </c>
-      <c r="K248" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="L248" s="40">
+      <c r="K248" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="L248">
         <v>0.72</v>
       </c>
-      <c r="M248" s="41">
+      <c r="M248" s="34">
         <v>0.77</v>
       </c>
     </row>
     <row r="249" spans="3:13">
-      <c r="C249" s="39"/>
-      <c r="D249" s="42">
+      <c r="C249" s="33"/>
+      <c r="D249" s="1">
         <f>AVERAGE(D244:D248)</f>
         <v>0.68799999999999994</v>
       </c>
-      <c r="E249" s="43">
+      <c r="E249" s="35">
         <f>AVERAGE(E244:E248)</f>
         <v>0.82399999999999984</v>
       </c>
-      <c r="G249" s="39"/>
-      <c r="H249" s="40">
+      <c r="G249" s="33"/>
+      <c r="H249">
         <v>0.73</v>
       </c>
-      <c r="I249" s="41">
+      <c r="I249" s="34">
         <v>0.8</v>
       </c>
-      <c r="K249" s="39"/>
-      <c r="L249" s="40">
+      <c r="K249" s="33"/>
+      <c r="L249">
         <v>0.72</v>
       </c>
-      <c r="M249" s="41">
+      <c r="M249" s="34">
         <v>0.77</v>
       </c>
     </row>
     <row r="250" spans="3:13">
-      <c r="C250" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D250" s="48">
+      <c r="C250" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250">
         <v>0.72</v>
       </c>
-      <c r="E250" s="50">
+      <c r="E250" s="34">
         <v>0.81</v>
       </c>
-      <c r="G250" s="39"/>
-      <c r="H250" s="40">
+      <c r="G250" s="33"/>
+      <c r="H250">
         <v>0.75</v>
       </c>
-      <c r="I250" s="41">
+      <c r="I250" s="34">
         <v>0.84</v>
       </c>
-      <c r="K250" s="39"/>
-      <c r="L250" s="40">
+      <c r="K250" s="33"/>
+      <c r="L250">
         <v>0.73</v>
       </c>
-      <c r="M250" s="41">
+      <c r="M250" s="34">
         <v>0.82</v>
       </c>
     </row>
     <row r="251" spans="3:13">
-      <c r="C251" s="39"/>
-      <c r="D251" s="47">
+      <c r="C251" s="33"/>
+      <c r="D251" s="39">
         <v>0.7</v>
       </c>
-      <c r="E251" s="49">
+      <c r="E251" s="40">
         <v>0.84</v>
       </c>
-      <c r="G251" s="44"/>
-      <c r="H251" s="45">
+      <c r="G251" s="36"/>
+      <c r="H251" s="37">
         <f>AVERAGE(H248:H250)</f>
         <v>0.7533333333333333</v>
       </c>
-      <c r="I251" s="46">
+      <c r="I251" s="38">
         <f>AVERAGE(I248:I250)</f>
         <v>0.82</v>
       </c>
-      <c r="K251" s="39"/>
-      <c r="L251" s="40">
+      <c r="K251" s="33"/>
+      <c r="L251">
         <v>0.79</v>
       </c>
-      <c r="M251" s="41">
+      <c r="M251" s="34">
         <v>0.76</v>
       </c>
     </row>
     <row r="252" spans="3:13">
-      <c r="C252" s="39"/>
-      <c r="D252" s="40">
+      <c r="C252" s="33"/>
+      <c r="D252">
         <v>0.71</v>
       </c>
-      <c r="E252" s="41">
+      <c r="E252" s="34">
         <v>0.74</v>
       </c>
-      <c r="K252" s="44"/>
-      <c r="L252" s="45">
+      <c r="K252" s="36"/>
+      <c r="L252" s="37">
         <f>AVERAGE(L248:L251)</f>
         <v>0.74</v>
       </c>
-      <c r="M252" s="46">
+      <c r="M252" s="38">
         <f>AVERAGE(M248:M251)</f>
         <v>0.78</v>
       </c>
     </row>
     <row r="253" spans="3:13">
-      <c r="C253" s="39"/>
-      <c r="D253" s="40">
+      <c r="C253" s="33"/>
+      <c r="D253">
         <v>0.74</v>
       </c>
-      <c r="E253" s="41">
+      <c r="E253" s="34">
         <v>0.82</v>
       </c>
     </row>
     <row r="254" spans="3:13">
-      <c r="C254" s="39"/>
-      <c r="D254" s="40">
+      <c r="C254" s="33"/>
+      <c r="D254">
         <v>0.75</v>
       </c>
-      <c r="E254" s="41">
+      <c r="E254" s="34">
         <v>0.73</v>
       </c>
     </row>
     <row r="255" spans="3:13">
-      <c r="C255" s="44"/>
-      <c r="D255" s="45">
+      <c r="C255" s="36"/>
+      <c r="D255" s="37">
         <f>AVERAGE(D250:D254)</f>
         <v>0.72399999999999998</v>
       </c>
-      <c r="E255" s="46">
+      <c r="E255" s="38">
         <f>AVERAGE(E250:E254)</f>
         <v>0.78799999999999992</v>
       </c>
@@ -4491,7 +4516,7 @@
         <v>0.72803643494844383</v>
       </c>
       <c r="E267" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G267" t="s">
         <v>216</v>
@@ -4510,9 +4535,9 @@
       <c r="C268" t="s">
         <v>224</v>
       </c>
-      <c r="D268" s="9">
-        <f>AVERAGE(F61:G61,F103:G103,F145:G145,F82:G82,F124:G124,)</f>
-        <v>0.59790209790209747</v>
+      <c r="D268" s="48">
+        <f>AVERAGE(F61:G61,F103:G103,F145:G145,F82:G82,F124:G124)</f>
+        <v>0.65769230769230724</v>
       </c>
       <c r="G268" t="s">
         <v>217</v>
@@ -4531,9 +4556,9 @@
       <c r="C269" t="s">
         <v>225</v>
       </c>
-      <c r="D269" s="9">
-        <f>AVERAGE(F63:G63,F84:G84,F105:G105,F126:G126,F147:G147,)</f>
-        <v>0.65509753404490212</v>
+      <c r="D269" s="48">
+        <f>AVERAGE(F63:G63,F84:G84,F105:G105,F126:G126,F147:G147)</f>
+        <v>0.72060728744939229</v>
       </c>
       <c r="G269" t="s">
         <v>218</v>
@@ -4616,9 +4641,9 @@
       <c r="C279" t="s">
         <v>229</v>
       </c>
-      <c r="D279" s="9">
-        <f>AVERAGE(D23:E23,F61:G61,F63:G63,F65:G65,)</f>
-        <v>0.63063427867837885</v>
+      <c r="D279" s="48">
+        <f>AVERAGE(D23:E23,F61:G61,F63:G63,F65:G65)</f>
+        <v>0.70946356351317619</v>
       </c>
       <c r="E279">
         <v>8</v>
@@ -4628,9 +4653,9 @@
       <c r="C280" t="s">
         <v>230</v>
       </c>
-      <c r="D280" s="9">
-        <f>AVERAGE(E78:F78,F82:G82,F84:G84,F86:G86,)</f>
-        <v>0.5609086815966603</v>
+      <c r="D280" s="48">
+        <f>AVERAGE(E78:F78,F82:G82,F84:G84,F86:G86)</f>
+        <v>0.63102226679624285</v>
       </c>
       <c r="E280">
         <v>8</v>
@@ -4664,9 +4689,9 @@
       <c r="C283" t="s">
         <v>233</v>
       </c>
-      <c r="D283" s="9">
-        <f>AVERAGE(F145:G145,F147:G147,E161:F161,E171:F171,)</f>
-        <v>0.6066276795164468</v>
+      <c r="D283" s="48">
+        <f>AVERAGE(F145:G145,F147:G147,E161:F161,E171:F171)</f>
+        <v>0.6824561394560027</v>
       </c>
       <c r="E283" t="s">
         <v>235</v>
@@ -4676,9 +4701,9 @@
       <c r="C284" t="s">
         <v>234</v>
       </c>
-      <c r="D284" s="9">
-        <f>AVERAGE(E201:F201,F205:G205,F207:G207,E221:F221,E235:F235,)</f>
-        <v>0.50198748587479713</v>
+      <c r="D284" s="48">
+        <f>AVERAGE(E201:F201,F205:G205,F207:G207,E221:F221,E235:F235)</f>
+        <v>0.55218623446227677</v>
       </c>
       <c r="E284" t="s">
         <v>236</v>
@@ -4686,11 +4711,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E203:G203"/>
-    <mergeCell ref="C205:C210"/>
-    <mergeCell ref="E164:G164"/>
-    <mergeCell ref="C166:C171"/>
-    <mergeCell ref="E188:G188"/>
     <mergeCell ref="E143:G143"/>
     <mergeCell ref="C145:C150"/>
     <mergeCell ref="C2:E2"/>
@@ -4703,6 +4723,11 @@
     <mergeCell ref="C82:C87"/>
     <mergeCell ref="E101:G101"/>
     <mergeCell ref="C103:C108"/>
+    <mergeCell ref="E203:G203"/>
+    <mergeCell ref="C205:C210"/>
+    <mergeCell ref="E164:G164"/>
+    <mergeCell ref="C166:C171"/>
+    <mergeCell ref="E188:G188"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>